<commit_message>
working vectorized version with one brand
</commit_message>
<xml_diff>
--- a/estimatedParametersMean.xlsx
+++ b/estimatedParametersMean.xlsx
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-248221.8386974035</v>
+        <v>328.315284925559</v>
       </c>
     </row>
     <row r="3">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.8746670212820963</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.008346681965080656</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>8.953749999999999</v>
       </c>
     </row>
     <row r="6">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>516.48375</v>
       </c>
     </row>
     <row r="7">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.0015</v>
       </c>
     </row>
     <row r="8">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>248249.6561166183</v>
+        <v>-300.946032084674</v>
       </c>
     </row>
     <row r="9">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.051267735176402</v>
+        <v>0.001332935949889836</v>
       </c>
     </row>
     <row r="10">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.06113424024430314</v>
+        <v>0.3495051709850945</v>
       </c>
     </row>
     <row r="11">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.2248182777941097</v>
+        <v>-0.02824679883403852</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-1.014897176661136</v>
+        <v>-0.03455585595111852</v>
       </c>
     </row>
     <row r="13">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.3237314037237786</v>
+        <v>-0.01986536232395531</v>
       </c>
     </row>
     <row r="14">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.2478661971709193</v>
+        <v>-0.009720857740090561</v>
       </c>
     </row>
     <row r="15">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.2536194593698129</v>
+        <v>0.05295825344168772</v>
       </c>
     </row>
     <row r="16">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.594278457159152</v>
+        <v>-0.002067417302561788</v>
       </c>
     </row>
     <row r="17">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9608629078763582</v>
+        <v>0.06011531524067524</v>
       </c>
     </row>
     <row r="18">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.216202222087137</v>
+        <v>0.05297351206418582</v>
       </c>
     </row>
     <row r="19">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.07751079586610587</v>
+        <v>0.006935702562776358</v>
       </c>
     </row>
     <row r="20">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-1.491893561697959</v>
+        <v>-0.02667817067807694</v>
       </c>
     </row>
     <row r="21">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.4543733816016982</v>
+        <v>-0.04728346606388122</v>
       </c>
     </row>
     <row r="22">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.7351880572858143</v>
+        <v>-0.01873515736007087</v>
       </c>
     </row>
     <row r="23">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-1.681568393770085</v>
+        <v>0.01829467878929958</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.194710152570658</v>
+        <v>0.02565852472165002</v>
       </c>
     </row>
     <row r="25">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.6379437906961729</v>
+        <v>0.01640572261186893</v>
       </c>
     </row>
     <row r="26">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.8112379507005514</v>
+        <v>0.01636145803295166</v>
       </c>
     </row>
     <row r="27">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-1.786936524173497</v>
+        <v>0.06225266487576391</v>
       </c>
     </row>
     <row r="28">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-1.453591196336245</v>
+        <v>0.01631401359848264</v>
       </c>
     </row>
     <row r="29">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.01243083601307671</v>
+        <v>0.02117164056326543</v>
       </c>
     </row>
     <row r="30">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-1.721995914397598</v>
+        <v>0.02852351669009486</v>
       </c>
     </row>
     <row r="31">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-1.600450957957088</v>
+        <v>0.001315472219804538</v>
       </c>
     </row>
     <row r="32">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.8291035198154408</v>
+        <v>2.433010894236689</v>
       </c>
     </row>
     <row r="33">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.9621809920051905</v>
+        <v>0.1613745064512964</v>
       </c>
     </row>
     <row r="34">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.761908183584038</v>
+        <v>0.001757668512869779</v>
       </c>
     </row>
     <row r="35">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.9273206366922588</v>
+        <v>0.0003337745490848469</v>
       </c>
     </row>
     <row r="36">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.5223459447863765</v>
+        <v>0.5545871550675672</v>
       </c>
     </row>
     <row r="37">
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.7011323520703061</v>
+        <v>0.472462981532121</v>
       </c>
     </row>
     <row r="38">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.7196492915898153</v>
+        <v>0.4764557776664566</v>
       </c>
     </row>
     <row r="39">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.4189344661917536</v>
+        <v>0.6383014200664587</v>
       </c>
     </row>
     <row r="40">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.4556654016647256</v>
+        <v>0.4340699122414538</v>
       </c>
     </row>
     <row r="41">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1859821545355301</v>
+        <v>0.4760302479310534</v>
       </c>
     </row>
     <row r="42">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.1411677130429406</v>
+        <v>0.4651697543742474</v>
       </c>
     </row>
     <row r="43">
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1.210522955084144</v>
+        <v>1.012602464670007</v>
       </c>
     </row>
     <row r="44">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1.30187771148999</v>
+        <v>0.9952153791251452</v>
       </c>
     </row>
     <row r="45">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1.752981216558422</v>
+        <v>1.002165228254549</v>
       </c>
     </row>
     <row r="46">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.3620536372165651</v>
+        <v>1.00454033212596</v>
       </c>
     </row>
     <row r="47">
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1.227161014811288</v>
+        <v>0.9872634899780622</v>
       </c>
     </row>
     <row r="48">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.3942369138953178</v>
+        <v>1.007177646466636</v>
       </c>
     </row>
     <row r="49">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1.648109320180658</v>
+        <v>0.9963717657605378</v>
       </c>
     </row>
     <row r="50">
@@ -930,7 +930,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.1483812248835406</v>
+        <v>0.8812743518639963</v>
       </c>
     </row>
     <row r="51">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.5943201027113832</v>
+        <v>0.9980362791383721</v>
       </c>
     </row>
     <row r="52">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.2215886309027454</v>
+        <v>0.9965251228081988</v>
       </c>
     </row>
     <row r="53">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1.386262649738986</v>
+        <v>0.6129622236257619</v>
       </c>
     </row>
     <row r="54">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1958276728709335</v>
+        <v>1.1139815397045</v>
       </c>
     </row>
     <row r="55">
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.2917519523352822</v>
+        <v>0.958973141006828</v>
       </c>
     </row>
     <row r="56">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.386072705009236</v>
+        <v>1.170041814237061</v>
       </c>
     </row>
     <row r="57">
@@ -1000,7 +1000,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.7485933787997769</v>
+        <v>0.5171060693220666</v>
       </c>
     </row>
     <row r="58">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.1738721930237854</v>
+        <v>0.5445130887041298</v>
       </c>
     </row>
     <row r="59">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.3040226523875741</v>
+        <v>0.5335528745396414</v>
       </c>
     </row>
     <row r="60">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.6212219122781149</v>
+        <v>0.4028003423538463</v>
       </c>
     </row>
     <row r="61">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.7037187774820656</v>
+        <v>0.5686431390833666</v>
       </c>
     </row>
     <row r="62">
@@ -1050,7 +1050,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.1218773610230654</v>
+        <v>0.5298702250507513</v>
       </c>
     </row>
     <row r="63">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.7446052977890089</v>
+        <v>0.5741825085750883</v>
       </c>
     </row>
     <row r="64">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.01123144480641655</v>
+        <v>0.1829427527346514</v>
       </c>
     </row>
     <row r="65">
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.0001453711662830974</v>
+        <v>0.1226332346159231</v>
       </c>
     </row>
     <row r="66">
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>0.09985366389750722</v>
       </c>
     </row>
     <row r="67">
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.002413557032756655</v>
+        <v>0.1741212829389117</v>
       </c>
     </row>
     <row r="68">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.001385730900785735</v>
+        <v>0.1448418638001618</v>
       </c>
     </row>
     <row r="69">
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.008166208143762739</v>
+        <v>0.2064183803009754</v>
       </c>
     </row>
     <row r="70">
@@ -1130,7 +1130,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.01239680595650853</v>
+        <v>0.2348448431037291</v>
       </c>
     </row>
     <row r="71">
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.003566215488090736</v>
+        <v>0.1894733585155782</v>
       </c>
     </row>
     <row r="72">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.01521103515215581</v>
+        <v>0.2487673717339593</v>
       </c>
     </row>
     <row r="73">
@@ -1160,7 +1160,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.01812315691391927</v>
+        <v>0.2586353299097324</v>
       </c>
     </row>
     <row r="74">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.006348133998333344</v>
+        <v>0.2112349287975822</v>
       </c>
     </row>
     <row r="75">
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.008294902874301036</v>
+        <v>0.2250714134972812</v>
       </c>
     </row>
     <row r="76">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.01321200748547035</v>
+        <v>0.2410574350604749</v>
       </c>
     </row>
     <row r="77">
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>9.358360826002177e-05</v>
+        <v>0.1529965853844491</v>
       </c>
     </row>
     <row r="78">
@@ -1210,7 +1210,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>0.1348353136519238</v>
       </c>
     </row>
     <row r="79">
@@ -1220,7 +1220,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>9.666506715757115e-05</v>
+        <v>0.1335018457112911</v>
       </c>
     </row>
     <row r="80">
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>0.03860779840296594</v>
       </c>
     </row>
     <row r="81">
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>0.01316558382506357</v>
       </c>
     </row>
     <row r="82">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0</v>
+        <v>0.008887986378223111</v>
       </c>
     </row>
     <row r="83">
@@ -1260,7 +1260,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0</v>
+        <v>0.02399694574334219</v>
       </c>
     </row>
     <row r="84">
@@ -1270,7 +1270,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.003009253868412787</v>
+        <v>0.1517107339170709</v>
       </c>
     </row>
     <row r="85">
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.0009000900766199881</v>
+        <v>0.1472723728136556</v>
       </c>
     </row>
     <row r="86">
@@ -1290,7 +1290,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0</v>
+        <v>0.09951948313719194</v>
       </c>
     </row>
     <row r="87">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>0.0790335487160935</v>
       </c>
     </row>
     <row r="88">
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>0.06154403377550107</v>
       </c>
     </row>
     <row r="89">
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0</v>
+        <v>0.02702976830527308</v>
       </c>
     </row>
     <row r="90">
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0</v>
+        <v>0.06618770914937953</v>
       </c>
     </row>
     <row r="91">
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>0.01924396195541494</v>
       </c>
     </row>
     <row r="92">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0</v>
+        <v>0.0001109230833151566</v>
       </c>
     </row>
     <row r="93">
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0</v>
+        <v>0.04791052888420236</v>
       </c>
     </row>
     <row r="108">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.01052127190973107</v>
+        <v>0.200607183738323</v>
       </c>
     </row>
     <row r="109">
@@ -1520,7 +1520,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.01795131710056618</v>
+        <v>0.2465209724435361</v>
       </c>
     </row>
     <row r="110">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.0214043923761725</v>
+        <v>0.2728869542741047</v>
       </c>
     </row>
     <row r="111">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.02278820687244879</v>
+        <v>0.2805750028195036</v>
       </c>
     </row>
     <row r="112">
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.02476936530223258</v>
+        <v>0.2859244943793271</v>
       </c>
     </row>
     <row r="113">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.02557517812382199</v>
+        <v>0.288534193313668</v>
       </c>
     </row>
     <row r="114">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.0258995885781607</v>
+        <v>0.2900919813738485</v>
       </c>
     </row>
     <row r="115">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.05838870054890088</v>
+        <v>0.3520730681010802</v>
       </c>
     </row>
     <row r="116">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.02740084242473385</v>
+        <v>0.2990296555203903</v>
       </c>
     </row>
     <row r="117">
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.01703046721017502</v>
+        <v>0.2725309585468516</v>
       </c>
     </row>
     <row r="118">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.01332266962741794</v>
+        <v>0.2572071685396967</v>
       </c>
     </row>
     <row r="119">
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.01134629784651834</v>
+        <v>0.2355654166444575</v>
       </c>
     </row>
     <row r="120">
@@ -1630,7 +1630,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.01134629784651834</v>
+        <v>0.2355654166444575</v>
       </c>
     </row>
     <row r="121">
@@ -1640,7 +1640,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0</v>
+        <v>0.1114840227893504</v>
       </c>
     </row>
     <row r="122">
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0</v>
+        <v>0.03625625165871538</v>
       </c>
     </row>
     <row r="123">
@@ -1660,7 +1660,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0</v>
+        <v>0.0001500727079621149</v>
       </c>
     </row>
     <row r="124">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.004243885667864318</v>
+        <v>0.1558207807015238</v>
       </c>
     </row>
     <row r="131">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0</v>
+        <v>0.09809761186430387</v>
       </c>
     </row>
     <row r="132">
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>0.04655262533703497</v>
       </c>
     </row>
     <row r="133">
@@ -1760,7 +1760,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0</v>
+        <v>0.007329214250668709</v>
       </c>
     </row>
     <row r="134">
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.06770389552286291</v>
+        <v>0.3371580934139399</v>
       </c>
     </row>
     <row r="162">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.3088024366852565</v>
+        <v>0.542269897242787</v>
       </c>
     </row>
     <row r="163">
@@ -2060,7 +2060,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.3860000004812463</v>
+        <v>0.5814927691488461</v>
       </c>
     </row>
     <row r="164">
@@ -2070,7 +2070,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.1111385622572787</v>
+        <v>0.4426279224690361</v>
       </c>
     </row>
     <row r="165">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.1548049454733083</v>
+        <v>0.486712024679967</v>
       </c>
     </row>
     <row r="166">
@@ -2090,7 +2090,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.2604540039670701</v>
+        <v>0.5349852701284062</v>
       </c>
     </row>
     <row r="167">
@@ -2100,7 +2100,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.3978372950041409</v>
+        <v>0.5853338486211206</v>
       </c>
     </row>
     <row r="168">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.2406652577195438</v>
+        <v>0.5260803610110101</v>
       </c>
     </row>
     <row r="169">
@@ -2120,7 +2120,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.05117668677550894</v>
+        <v>0.3883847389969767</v>
       </c>
     </row>
     <row r="170">
@@ -2130,7 +2130,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.04616834309789167</v>
+        <v>0.376132394417572</v>
       </c>
     </row>
     <row r="171">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.08913429593863235</v>
+        <v>0.3947767074936018</v>
       </c>
     </row>
     <row r="172">
@@ -2150,7 +2150,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.1215220417411699</v>
+        <v>0.4265031715158638</v>
       </c>
     </row>
     <row r="173">
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.1407418986708938</v>
+        <v>0.4549567952136551</v>
       </c>
     </row>
     <row r="174">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.145576827335647</v>
+        <v>0.4630601535980877</v>
       </c>
     </row>
     <row r="175">
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.02037682938338243</v>
+        <v>0.3098965133224975</v>
       </c>
     </row>
     <row r="176">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>8.66167692750296e-10</v>
+        <v>0.2089584807517089</v>
       </c>
     </row>
     <row r="177">
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0</v>
+        <v>0.104395853765098</v>
       </c>
     </row>
     <row r="178">
@@ -2330,7 +2330,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.02005435025182987</v>
+        <v>0.2335766386007191</v>
       </c>
     </row>
     <row r="191">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.04933926696206509</v>
+        <v>0.3226975670756355</v>
       </c>
     </row>
     <row r="192">
@@ -2350,7 +2350,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.08274855473405361</v>
+        <v>0.3863241491088383</v>
       </c>
     </row>
     <row r="193">
@@ -2360,7 +2360,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.005922546193359832</v>
+        <v>0.2438729768333606</v>
       </c>
     </row>
     <row r="194">
@@ -2370,7 +2370,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0</v>
+        <v>0.1382758692738851</v>
       </c>
     </row>
     <row r="195">
@@ -2380,7 +2380,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0</v>
+        <v>0.04367694507818101</v>
       </c>
     </row>
     <row r="196">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0</v>
+        <v>0.003485938026321081</v>
       </c>
     </row>
     <row r="214">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0.02284441593025157</v>
+        <v>0.2413638997179827</v>
       </c>
     </row>
     <row r="217">
@@ -2600,7 +2600,7 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.1690102878641993</v>
+        <v>0.4559115644827267</v>
       </c>
     </row>
     <row r="218">
@@ -2610,7 +2610,7 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.2336958173427189</v>
+        <v>0.5109303684465051</v>
       </c>
     </row>
     <row r="219">
@@ -2620,7 +2620,7 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.385017169057722</v>
+        <v>0.583822049682878</v>
       </c>
     </row>
     <row r="220">
@@ -2630,7 +2630,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.3037234534228402</v>
+        <v>0.555781271457325</v>
       </c>
     </row>
     <row r="221">
@@ -2670,7 +2670,7 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.3471366298834515</v>
+        <v>0.1457818846177044</v>
       </c>
     </row>
     <row r="225">
@@ -2680,7 +2680,7 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.4461233311025956</v>
+        <v>0.1984167010342177</v>
       </c>
     </row>
     <row r="226">
@@ -2690,7 +2690,7 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.4361791610594454</v>
+        <v>0.1481204108987429</v>
       </c>
     </row>
     <row r="227">
@@ -2700,7 +2700,7 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.440417771552988</v>
+        <v>0.1587970790487397</v>
       </c>
     </row>
     <row r="228">
@@ -2710,7 +2710,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.2804545265520095</v>
+        <v>0.04829502529892376</v>
       </c>
     </row>
     <row r="229">
@@ -2720,7 +2720,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0</v>
+        <v>0.006207399796177952</v>
       </c>
     </row>
     <row r="230">
@@ -2840,7 +2840,7 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>0.2008401604381603</v>
+        <v>0.06039796137709019</v>
       </c>
     </row>
     <row r="242">
@@ -2850,7 +2850,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.2256192001962714</v>
+        <v>0.04125959903395689</v>
       </c>
     </row>
     <row r="243">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0</v>
+        <v>0.01110337210282745</v>
       </c>
     </row>
     <row r="244">
@@ -2870,7 +2870,7 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>0</v>
+        <v>0.002261588413446722</v>
       </c>
     </row>
     <row r="245">
@@ -3090,7 +3090,7 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>0.5582060163674687</v>
+        <v>0.3645685288955337</v>
       </c>
     </row>
     <row r="267">
@@ -3100,7 +3100,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>0.6338263236446753</v>
+        <v>0.4881625344364357</v>
       </c>
     </row>
     <row r="268">
@@ -3110,7 +3110,7 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>0.6405738022760108</v>
+        <v>0.4633398285573013</v>
       </c>
     </row>
     <row r="269">
@@ -3120,7 +3120,7 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.6153192091443187</v>
+        <v>0.3290271000316161</v>
       </c>
     </row>
     <row r="270">
@@ -3130,7 +3130,7 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.5636651060601837</v>
+        <v>0.2337714456658564</v>
       </c>
     </row>
     <row r="271">
@@ -3140,7 +3140,7 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>0.4639698739015444</v>
+        <v>0.1515378813934546</v>
       </c>
     </row>
     <row r="272">
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.3596509856966973</v>
+        <v>0.1017313649851173</v>
       </c>
     </row>
     <row r="273">
@@ -3160,7 +3160,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.1540725279434861</v>
+        <v>0.02638444101572861</v>
       </c>
     </row>
     <row r="274">
@@ -3170,7 +3170,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0</v>
+        <v>0.003730865279381802</v>
       </c>
     </row>
     <row r="275">
@@ -3310,7 +3310,7 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>0</v>
+        <v>0.001307599475877211</v>
       </c>
     </row>
     <row r="289">
@@ -3320,7 +3320,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>0</v>
+        <v>0.0005873903630659458</v>
       </c>
     </row>
     <row r="290">
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="B322" t="n">
-        <v>0.4523165906682122</v>
+        <v>0.2444945646421943</v>
       </c>
     </row>
     <row r="323">
@@ -3660,7 +3660,7 @@
         </is>
       </c>
       <c r="B323" t="n">
-        <v>0.550420763825091</v>
+        <v>0.3266038078297744</v>
       </c>
     </row>
     <row r="324">
@@ -3670,7 +3670,7 @@
         </is>
       </c>
       <c r="B324" t="n">
-        <v>0.5863208298153948</v>
+        <v>0.3606578134767405</v>
       </c>
     </row>
     <row r="325">
@@ -3680,7 +3680,7 @@
         </is>
       </c>
       <c r="B325" t="n">
-        <v>0.5608629354304592</v>
+        <v>0.2599187394648499</v>
       </c>
     </row>
     <row r="326">
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="B326" t="n">
-        <v>0.4600664830414245</v>
+        <v>0.1203139392189302</v>
       </c>
     </row>
     <row r="327">
@@ -3700,7 +3700,7 @@
         </is>
       </c>
       <c r="B327" t="n">
-        <v>0.4103889190061484</v>
+        <v>0.1251762327451833</v>
       </c>
     </row>
     <row r="328">
@@ -3710,7 +3710,7 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>0.3609832026420757</v>
+        <v>0.1251585028949456</v>
       </c>
     </row>
     <row r="329">
@@ -3720,7 +3720,7 @@
         </is>
       </c>
       <c r="B329" t="n">
-        <v>0.3886968148992901</v>
+        <v>0.1394629872582267</v>
       </c>
     </row>
     <row r="330">
@@ -3730,7 +3730,7 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>0.4251823923518495</v>
+        <v>0.1554092637781167</v>
       </c>
     </row>
     <row r="331">
@@ -3740,7 +3740,7 @@
         </is>
       </c>
       <c r="B331" t="n">
-        <v>0.4251823923518495</v>
+        <v>0.1554092637781167</v>
       </c>
     </row>
     <row r="332">
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="B332" t="n">
-        <v>0.2775324516540689</v>
+        <v>0.04763473092700469</v>
       </c>
     </row>
     <row r="333">
@@ -3760,7 +3760,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>0</v>
+        <v>0.01124683780999495</v>
       </c>
     </row>
     <row r="334">
@@ -4160,7 +4160,7 @@
         </is>
       </c>
       <c r="B373" t="n">
-        <v>0.4533609832299034</v>
+        <v>0.2455022202369688</v>
       </c>
     </row>
     <row r="374">
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="B374" t="n">
-        <v>0.5650912930546236</v>
+        <v>0.3525230688299579</v>
       </c>
     </row>
     <row r="375">
@@ -4180,7 +4180,7 @@
         </is>
       </c>
       <c r="B375" t="n">
-        <v>0.6018203296136297</v>
+        <v>0.3922460962295746</v>
       </c>
     </row>
     <row r="376">
@@ -4190,7 +4190,7 @@
         </is>
       </c>
       <c r="B376" t="n">
-        <v>0.6191701387712107</v>
+        <v>0.4109433517099328</v>
       </c>
     </row>
     <row r="377">
@@ -4200,7 +4200,7 @@
         </is>
       </c>
       <c r="B377" t="n">
-        <v>0.5926090087088939</v>
+        <v>0.3235357205667821</v>
       </c>
     </row>
     <row r="378">
@@ -5740,7 +5740,7 @@
         </is>
       </c>
       <c r="B531" t="n">
-        <v>0.4988349329584199</v>
+        <v>0.4208361588607124</v>
       </c>
     </row>
     <row r="532">
@@ -5750,7 +5750,7 @@
         </is>
       </c>
       <c r="B532" t="n">
-        <v>0.5317228653584998</v>
+        <v>0.5206075299665146</v>
       </c>
     </row>
     <row r="533">
@@ -5760,7 +5760,7 @@
         </is>
       </c>
       <c r="B533" t="n">
-        <v>0.5511646200575224</v>
+        <v>0.5758568320782456</v>
       </c>
     </row>
     <row r="534">
@@ -5770,7 +5770,7 @@
         </is>
       </c>
       <c r="B534" t="n">
-        <v>0.5496952514536891</v>
+        <v>0.5252953984132142</v>
       </c>
     </row>
     <row r="535">
@@ -5780,7 +5780,7 @@
         </is>
       </c>
       <c r="B535" t="n">
-        <v>0.09188731582289315</v>
+        <v>0.3875596101597393</v>
       </c>
     </row>
     <row r="536">
@@ -5790,7 +5790,7 @@
         </is>
       </c>
       <c r="B536" t="n">
-        <v>0.01444440552072027</v>
+        <v>0.3075265386672704</v>
       </c>
     </row>
     <row r="537">
@@ -5800,7 +5800,7 @@
         </is>
       </c>
       <c r="B537" t="n">
-        <v>0</v>
+        <v>0.2218306678424999</v>
       </c>
     </row>
     <row r="538">
@@ -5810,7 +5810,7 @@
         </is>
       </c>
       <c r="B538" t="n">
-        <v>0</v>
+        <v>0.1569917160954336</v>
       </c>
     </row>
     <row r="539">
@@ -5880,7 +5880,7 @@
         </is>
       </c>
       <c r="B545" t="n">
-        <v>0.02484952371287668</v>
+        <v>0.2811676504345905</v>
       </c>
     </row>
     <row r="546">
@@ -5890,7 +5890,7 @@
         </is>
       </c>
       <c r="B546" t="n">
-        <v>0.02978242678421961</v>
+        <v>0.3242526612000631</v>
       </c>
     </row>
     <row r="547">
@@ -5900,7 +5900,7 @@
         </is>
       </c>
       <c r="B547" t="n">
-        <v>0.09238342794714713</v>
+        <v>0.4131901953665488</v>
       </c>
     </row>
     <row r="548">
@@ -5910,7 +5910,7 @@
         </is>
       </c>
       <c r="B548" t="n">
-        <v>0.01458124435026241</v>
+        <v>0.3346477894940158</v>
       </c>
     </row>
     <row r="549">
@@ -5920,7 +5920,7 @@
         </is>
       </c>
       <c r="B549" t="n">
-        <v>0</v>
+        <v>0.2214138596085108</v>
       </c>
     </row>
     <row r="550">
@@ -5930,7 +5930,7 @@
         </is>
       </c>
       <c r="B550" t="n">
-        <v>0</v>
+        <v>0.1139181408073408</v>
       </c>
     </row>
     <row r="551">
@@ -6750,7 +6750,7 @@
         </is>
       </c>
       <c r="B632" t="n">
-        <v>0.04916590362378508</v>
+        <v>0.3338810880456111</v>
       </c>
     </row>
     <row r="633">
@@ -6760,7 +6760,7 @@
         </is>
       </c>
       <c r="B633" t="n">
-        <v>0.2783432978766322</v>
+        <v>0.5001386328356453</v>
       </c>
     </row>
     <row r="634">
@@ -6770,7 +6770,7 @@
         </is>
       </c>
       <c r="B634" t="n">
-        <v>0.4189544415497506</v>
+        <v>0.5513983053162581</v>
       </c>
     </row>
     <row r="635">
@@ -6780,7 +6780,7 @@
         </is>
       </c>
       <c r="B635" t="n">
-        <v>0.1601386089712102</v>
+        <v>0.4924286223387997</v>
       </c>
     </row>
     <row r="636">
@@ -6790,7 +6790,7 @@
         </is>
       </c>
       <c r="B636" t="n">
-        <v>0.420291315630359</v>
+        <v>0.5602637215574972</v>
       </c>
     </row>
     <row r="637">
@@ -6800,7 +6800,7 @@
         </is>
       </c>
       <c r="B637" t="n">
-        <v>0.4912317898339155</v>
+        <v>0.5755712227769241</v>
       </c>
     </row>
     <row r="638">
@@ -6810,7 +6810,7 @@
         </is>
       </c>
       <c r="B638" t="n">
-        <v>0.5147545218032753</v>
+        <v>0.5814903121012898</v>
       </c>
     </row>
     <row r="639">
@@ -6820,7 +6820,7 @@
         </is>
       </c>
       <c r="B639" t="n">
-        <v>0.3412961326029616</v>
+        <v>0.5537103914025511</v>
       </c>
     </row>
     <row r="640">
@@ -6830,7 +6830,7 @@
         </is>
       </c>
       <c r="B640" t="n">
-        <v>0.1014854298602317</v>
+        <v>0.4784528025564476</v>
       </c>
     </row>
     <row r="641">
@@ -6840,7 +6840,7 @@
         </is>
       </c>
       <c r="B641" t="n">
-        <v>0.1837024861220592</v>
+        <v>0.4960699052194424</v>
       </c>
     </row>
     <row r="642">
@@ -6850,7 +6850,7 @@
         </is>
       </c>
       <c r="B642" t="n">
-        <v>0.2644142870354858</v>
+        <v>0.5073035685577877</v>
       </c>
     </row>
     <row r="643">
@@ -6860,7 +6860,7 @@
         </is>
       </c>
       <c r="B643" t="n">
-        <v>0.3064455650741399</v>
+        <v>0.5245806157839301</v>
       </c>
     </row>
     <row r="644">
@@ -6870,7 +6870,7 @@
         </is>
       </c>
       <c r="B644" t="n">
-        <v>0.3226162090547906</v>
+        <v>0.5369419720904917</v>
       </c>
     </row>
     <row r="645">
@@ -6880,7 +6880,7 @@
         </is>
       </c>
       <c r="B645" t="n">
-        <v>0.3228363838344754</v>
+        <v>0.5383972022413843</v>
       </c>
     </row>
     <row r="646">
@@ -6890,7 +6890,7 @@
         </is>
       </c>
       <c r="B646" t="n">
-        <v>0.09809919927504498</v>
+        <v>0.4644336243989935</v>
       </c>
     </row>
     <row r="647">
@@ -6900,7 +6900,7 @@
         </is>
       </c>
       <c r="B647" t="n">
-        <v>0.01126779484418363</v>
+        <v>0.3636607402568181</v>
       </c>
     </row>
     <row r="648">
@@ -6910,7 +6910,7 @@
         </is>
       </c>
       <c r="B648" t="n">
-        <v>0</v>
+        <v>0.2260611105749523</v>
       </c>
     </row>
     <row r="649">
@@ -7300,7 +7300,7 @@
         </is>
       </c>
       <c r="B687" t="n">
-        <v>0.05736230030571622</v>
+        <v>0.3466834138482609</v>
       </c>
     </row>
     <row r="688">
@@ -7310,7 +7310,7 @@
         </is>
       </c>
       <c r="B688" t="n">
-        <v>0.3481048144571744</v>
+        <v>0.5227466513851668</v>
       </c>
     </row>
     <row r="689">
@@ -7320,7 +7320,7 @@
         </is>
       </c>
       <c r="B689" t="n">
-        <v>0.3798049865611794</v>
+        <v>0.544241641601745</v>
       </c>
     </row>
     <row r="690">
@@ -7330,7 +7330,7 @@
         </is>
       </c>
       <c r="B690" t="n">
-        <v>0.5185211490809454</v>
+        <v>0.5813878099284545</v>
       </c>
     </row>
     <row r="691">
@@ -7340,7 +7340,7 @@
         </is>
       </c>
       <c r="B691" t="n">
-        <v>0.5600487174160207</v>
+        <v>0.5941797251967949</v>
       </c>
     </row>
     <row r="692">
@@ -7370,7 +7370,7 @@
         </is>
       </c>
       <c r="B694" t="n">
-        <v>0.323178157636463</v>
+        <v>0.06583968135025371</v>
       </c>
     </row>
     <row r="695">
@@ -7380,7 +7380,7 @@
         </is>
       </c>
       <c r="B695" t="n">
-        <v>0</v>
+        <v>0.008788952490382888</v>
       </c>
     </row>
     <row r="696">
@@ -7390,7 +7390,7 @@
         </is>
       </c>
       <c r="B696" t="n">
-        <v>0</v>
+        <v>0.003416812610890638</v>
       </c>
     </row>
     <row r="697">
@@ -7400,7 +7400,7 @@
         </is>
       </c>
       <c r="B697" t="n">
-        <v>0</v>
+        <v>0.001737249377176469</v>
       </c>
     </row>
     <row r="698">
@@ -7770,7 +7770,7 @@
         </is>
       </c>
       <c r="B734" t="n">
-        <v>0.4077929180860275</v>
+        <v>0.1971331280001614</v>
       </c>
     </row>
     <row r="735">
@@ -7780,7 +7780,7 @@
         </is>
       </c>
       <c r="B735" t="n">
-        <v>0.462533486298325</v>
+        <v>0.3993221109713285</v>
       </c>
     </row>
     <row r="736">
@@ -7790,7 +7790,7 @@
         </is>
       </c>
       <c r="B736" t="n">
-        <v>0.4700929981666943</v>
+        <v>0.4285625126583716</v>
       </c>
     </row>
     <row r="737">
@@ -7800,7 +7800,7 @@
         </is>
       </c>
       <c r="B737" t="n">
-        <v>0.4412254429347779</v>
+        <v>0.2924184692588355</v>
       </c>
     </row>
     <row r="738">
@@ -7810,7 +7810,7 @@
         </is>
       </c>
       <c r="B738" t="n">
-        <v>0.4296139675770426</v>
+        <v>0.2701756440930621</v>
       </c>
     </row>
     <row r="739">
@@ -7820,7 +7820,7 @@
         </is>
       </c>
       <c r="B739" t="n">
-        <v>0.4378952880023799</v>
+        <v>0.300262038474824</v>
       </c>
     </row>
     <row r="740">
@@ -7830,7 +7830,7 @@
         </is>
       </c>
       <c r="B740" t="n">
-        <v>0.4547934283997874</v>
+        <v>0.3629792760494523</v>
       </c>
     </row>
     <row r="741">
@@ -7840,7 +7840,7 @@
         </is>
       </c>
       <c r="B741" t="n">
-        <v>0.4472774272730193</v>
+        <v>0.3254842865344711</v>
       </c>
     </row>
     <row r="742">
@@ -7850,7 +7850,7 @@
         </is>
       </c>
       <c r="B742" t="n">
-        <v>0.4297275836262416</v>
+        <v>0.2630928022933329</v>
       </c>
     </row>
     <row r="743">
@@ -7860,7 +7860,7 @@
         </is>
       </c>
       <c r="B743" t="n">
-        <v>0.3964752688257305</v>
+        <v>0.1740480475308392</v>
       </c>
     </row>
     <row r="744">
@@ -7870,7 +7870,7 @@
         </is>
       </c>
       <c r="B744" t="n">
-        <v>0.3720686315897851</v>
+        <v>0.1315963543755392</v>
       </c>
     </row>
     <row r="745">
@@ -7880,7 +7880,7 @@
         </is>
       </c>
       <c r="B745" t="n">
-        <v>0</v>
+        <v>0.04448465792480837</v>
       </c>
     </row>
     <row r="746">
@@ -7890,7 +7890,7 @@
         </is>
       </c>
       <c r="B746" t="n">
-        <v>0</v>
+        <v>0.00854126736486248</v>
       </c>
     </row>
     <row r="747">
@@ -7900,7 +7900,7 @@
         </is>
       </c>
       <c r="B747" t="n">
-        <v>0</v>
+        <v>0.0003132753149465464</v>
       </c>
     </row>
     <row r="748">
@@ -7950,7 +7950,7 @@
         </is>
       </c>
       <c r="B752" t="n">
-        <v>0.4278449345074725</v>
+        <v>0.25816186382897</v>
       </c>
     </row>
     <row r="753">
@@ -7960,7 +7960,7 @@
         </is>
       </c>
       <c r="B753" t="n">
-        <v>0.3808531723542993</v>
+        <v>0.1253823002059739</v>
       </c>
     </row>
     <row r="754">
@@ -7970,7 +7970,7 @@
         </is>
       </c>
       <c r="B754" t="n">
-        <v>0.3036501583523123</v>
+        <v>0.06727585776539627</v>
       </c>
     </row>
     <row r="755">
@@ -7980,7 +7980,7 @@
         </is>
       </c>
       <c r="B755" t="n">
-        <v>0</v>
+        <v>0.04103398945662414</v>
       </c>
     </row>
     <row r="756">
@@ -8000,7 +8000,7 @@
         </is>
       </c>
       <c r="B757" t="n">
-        <v>0.3183664187862069</v>
+        <v>0.0620296805970608</v>
       </c>
     </row>
     <row r="758">
@@ -8010,7 +8010,7 @@
         </is>
       </c>
       <c r="B758" t="n">
-        <v>0</v>
+        <v>0.007426109577957794</v>
       </c>
     </row>
     <row r="759">
@@ -8020,7 +8020,7 @@
         </is>
       </c>
       <c r="B759" t="n">
-        <v>0</v>
+        <v>0.002840393986640634</v>
       </c>
     </row>
     <row r="760">
@@ -8030,7 +8030,7 @@
         </is>
       </c>
       <c r="B760" t="n">
-        <v>0</v>
+        <v>0.001475923877196905</v>
       </c>
     </row>
     <row r="761">
@@ -8550,7 +8550,7 @@
         </is>
       </c>
       <c r="B812" t="n">
-        <v>0.358093006835024</v>
+        <v>0.1023607895011589</v>
       </c>
     </row>
     <row r="813">
@@ -8560,7 +8560,7 @@
         </is>
       </c>
       <c r="B813" t="n">
-        <v>0</v>
+        <v>0.02818708829146166</v>
       </c>
     </row>
     <row r="814">
@@ -8570,7 +8570,7 @@
         </is>
       </c>
       <c r="B814" t="n">
-        <v>0</v>
+        <v>0.01110107424949538</v>
       </c>
     </row>
     <row r="815">
@@ -8580,7 +8580,7 @@
         </is>
       </c>
       <c r="B815" t="n">
-        <v>0</v>
+        <v>0.006604683678629463</v>
       </c>
     </row>
     <row r="816">
@@ -8870,7 +8870,7 @@
         </is>
       </c>
       <c r="B844" t="n">
-        <v>0.4405612621869973</v>
+        <v>0.3056239672077384</v>
       </c>
     </row>
     <row r="845">
@@ -8880,7 +8880,7 @@
         </is>
       </c>
       <c r="B845" t="n">
-        <v>0.4218585282343998</v>
+        <v>0.2277787341280018</v>
       </c>
     </row>
     <row r="846">
@@ -8890,7 +8890,7 @@
         </is>
       </c>
       <c r="B846" t="n">
-        <v>0.4563710026318571</v>
+        <v>0.3730353343068085</v>
       </c>
     </row>
     <row r="847">
@@ -8900,7 +8900,7 @@
         </is>
       </c>
       <c r="B847" t="n">
-        <v>0.4474978900956816</v>
+        <v>0.3278968585636744</v>
       </c>
     </row>
     <row r="848">
@@ -8910,7 +8910,7 @@
         </is>
       </c>
       <c r="B848" t="n">
-        <v>0.4722233975153568</v>
+        <v>0.4470273534454801</v>
       </c>
     </row>
     <row r="849">
@@ -8940,7 +8940,7 @@
         </is>
       </c>
       <c r="B851" t="n">
-        <v>0.5380240664441847</v>
+        <v>0.3670246093265535</v>
       </c>
     </row>
     <row r="852">
@@ -8950,7 +8950,7 @@
         </is>
       </c>
       <c r="B852" t="n">
-        <v>0.3068707896986972</v>
+        <v>0.2051682079725347</v>
       </c>
     </row>
     <row r="853">
@@ -8960,7 +8960,7 @@
         </is>
       </c>
       <c r="B853" t="n">
-        <v>0</v>
+        <v>0.1343137661700478</v>
       </c>
     </row>
     <row r="854">
@@ -8970,7 +8970,7 @@
         </is>
       </c>
       <c r="B854" t="n">
-        <v>0.533450136718181</v>
+        <v>0.3873085540080645</v>
       </c>
     </row>
     <row r="855">
@@ -8980,7 +8980,7 @@
         </is>
       </c>
       <c r="B855" t="n">
-        <v>0.4301305641969175</v>
+        <v>0.2521714391592808</v>
       </c>
     </row>
     <row r="856">
@@ -8990,7 +8990,7 @@
         </is>
       </c>
       <c r="B856" t="n">
-        <v>0</v>
+        <v>0.130579680691564</v>
       </c>
     </row>
     <row r="857">
@@ -9000,7 +9000,7 @@
         </is>
       </c>
       <c r="B857" t="n">
-        <v>0</v>
+        <v>0.06530903838862392</v>
       </c>
     </row>
     <row r="858">
@@ -9390,7 +9390,7 @@
         </is>
       </c>
       <c r="B896" t="n">
-        <v>0.5780397323440956</v>
+        <v>0.4933012908678861</v>
       </c>
     </row>
     <row r="897">
@@ -9400,7 +9400,7 @@
         </is>
       </c>
       <c r="B897" t="n">
-        <v>0.4375134729066332</v>
+        <v>0.3154098785613499</v>
       </c>
     </row>
     <row r="898">
@@ -9410,7 +9410,7 @@
         </is>
       </c>
       <c r="B898" t="n">
-        <v>0</v>
+        <v>0.1896276876700147</v>
       </c>
     </row>
     <row r="899">
@@ -9420,7 +9420,7 @@
         </is>
       </c>
       <c r="B899" t="n">
-        <v>0.5400909003408882</v>
+        <v>0.4209165017360004</v>
       </c>
     </row>
     <row r="900">
@@ -9430,7 +9430,7 @@
         </is>
       </c>
       <c r="B900" t="n">
-        <v>0.3143919741547131</v>
+        <v>0.2048868618150815</v>
       </c>
     </row>
     <row r="901">
@@ -9440,7 +9440,7 @@
         </is>
       </c>
       <c r="B901" t="n">
-        <v>0.558426891872038</v>
+        <v>0.4611831958151973</v>
       </c>
     </row>
     <row r="902">
@@ -9450,7 +9450,7 @@
         </is>
       </c>
       <c r="B902" t="n">
-        <v>0.3894155190778134</v>
+        <v>0.2888126821938034</v>
       </c>
     </row>
     <row r="903">
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="B903" t="n">
-        <v>0</v>
+        <v>0.1378337773430828</v>
       </c>
     </row>
     <row r="904">
@@ -9470,7 +9470,7 @@
         </is>
       </c>
       <c r="B904" t="n">
-        <v>0</v>
+        <v>0.07649424949008904</v>
       </c>
     </row>
     <row r="905">
@@ -9480,7 +9480,7 @@
         </is>
       </c>
       <c r="B905" t="n">
-        <v>0.461925449957528</v>
+        <v>0.1945773823758435</v>
       </c>
     </row>
     <row r="906">
@@ -9490,7 +9490,7 @@
         </is>
       </c>
       <c r="B906" t="n">
-        <v>0.4899522020977064</v>
+        <v>0.2821914282751983</v>
       </c>
     </row>
     <row r="907">
@@ -9500,7 +9500,7 @@
         </is>
       </c>
       <c r="B907" t="n">
-        <v>0</v>
+        <v>0.1414445306924614</v>
       </c>
     </row>
     <row r="908">
@@ -9510,7 +9510,7 @@
         </is>
       </c>
       <c r="B908" t="n">
-        <v>0</v>
+        <v>0.06642617095420522</v>
       </c>
     </row>
     <row r="909">
@@ -9520,7 +9520,7 @@
         </is>
       </c>
       <c r="B909" t="n">
-        <v>0</v>
+        <v>0.01641994923566449</v>
       </c>
     </row>
     <row r="910">
@@ -9930,7 +9930,7 @@
         </is>
       </c>
       <c r="B950" t="n">
-        <v>0.5930506769655284</v>
+        <v>0.5440871964366909</v>
       </c>
     </row>
     <row r="951">
@@ -9940,7 +9940,7 @@
         </is>
       </c>
       <c r="B951" t="n">
-        <v>0.4679351431798574</v>
+        <v>0.3675987314594888</v>
       </c>
     </row>
     <row r="952">
@@ -9950,7 +9950,7 @@
         </is>
       </c>
       <c r="B952" t="n">
-        <v>0</v>
+        <v>0.2329128309866542</v>
       </c>
     </row>
     <row r="953">
@@ -9960,7 +9960,7 @@
         </is>
       </c>
       <c r="B953" t="n">
-        <v>0</v>
+        <v>0.1431669614620946</v>
       </c>
     </row>
     <row r="954">
@@ -9970,7 +9970,7 @@
         </is>
       </c>
       <c r="B954" t="n">
-        <v>0.5075323248502859</v>
+        <v>0.2831079314591862</v>
       </c>
     </row>
     <row r="955">
@@ -9980,7 +9980,7 @@
         </is>
       </c>
       <c r="B955" t="n">
-        <v>0.4133901931972955</v>
+        <v>0.2131953885019501</v>
       </c>
     </row>
     <row r="956">
@@ -9990,7 +9990,7 @@
         </is>
       </c>
       <c r="B956" t="n">
-        <v>0.5182334946131488</v>
+        <v>0.3572085699854409</v>
       </c>
     </row>
     <row r="957">
@@ -10000,7 +10000,7 @@
         </is>
       </c>
       <c r="B957" t="n">
-        <v>0.5577491402316891</v>
+        <v>0.4728221414859172</v>
       </c>
     </row>
     <row r="958">
@@ -10010,7 +10010,7 @@
         </is>
       </c>
       <c r="B958" t="n">
-        <v>0.3868179646199221</v>
+        <v>0.2877974831859422</v>
       </c>
     </row>
     <row r="959">
@@ -10020,7 +10020,7 @@
         </is>
       </c>
       <c r="B959" t="n">
-        <v>0</v>
+        <v>0.1668804219398008</v>
       </c>
     </row>
     <row r="960">
@@ -10030,7 +10030,7 @@
         </is>
       </c>
       <c r="B960" t="n">
-        <v>0</v>
+        <v>0.06771541127842616</v>
       </c>
     </row>
     <row r="961">
@@ -10040,7 +10040,7 @@
         </is>
       </c>
       <c r="B961" t="n">
-        <v>0.3504021034224248</v>
+        <v>0.0807537070549323</v>
       </c>
     </row>
     <row r="962">
@@ -10050,7 +10050,7 @@
         </is>
       </c>
       <c r="B962" t="n">
-        <v>0</v>
+        <v>0.004277414960263837</v>
       </c>
     </row>
     <row r="963">
@@ -10060,7 +10060,7 @@
         </is>
       </c>
       <c r="B963" t="n">
-        <v>0</v>
+        <v>0.00131951844027076</v>
       </c>
     </row>
     <row r="964">
@@ -10070,7 +10070,7 @@
         </is>
       </c>
       <c r="B964" t="n">
-        <v>0</v>
+        <v>0.0006959828910178837</v>
       </c>
     </row>
     <row r="965">
@@ -10450,7 +10450,7 @@
         </is>
       </c>
       <c r="B1002" t="n">
-        <v>0.3004861482098564</v>
+        <v>0.05524685068837701</v>
       </c>
     </row>
     <row r="1003">
@@ -10460,7 +10460,7 @@
         </is>
       </c>
       <c r="B1003" t="n">
-        <v>0</v>
+        <v>0.00082810805808801</v>
       </c>
     </row>
     <row r="1004">
@@ -10470,7 +10470,7 @@
         </is>
       </c>
       <c r="B1004" t="n">
-        <v>0.5738761141653677</v>
+        <v>0.4843459406249068</v>
       </c>
     </row>
     <row r="1005">
@@ -10480,7 +10480,7 @@
         </is>
       </c>
       <c r="B1005" t="n">
-        <v>0.4283434829345403</v>
+        <v>0.3072269273673418</v>
       </c>
     </row>
     <row r="1006">
@@ -10970,7 +10970,7 @@
         </is>
       </c>
       <c r="B1054" t="n">
-        <v>0.2673657512192599</v>
+        <v>0.1149068161009116</v>
       </c>
     </row>
     <row r="1055">
@@ -10980,7 +10980,7 @@
         </is>
       </c>
       <c r="B1055" t="n">
-        <v>0</v>
+        <v>0.03457901314419628</v>
       </c>
     </row>
     <row r="1056">
@@ -10990,7 +10990,7 @@
         </is>
       </c>
       <c r="B1056" t="n">
-        <v>0</v>
+        <v>0.01537280879465955</v>
       </c>
     </row>
     <row r="1057">
@@ -11000,7 +11000,7 @@
         </is>
       </c>
       <c r="B1057" t="n">
-        <v>0</v>
+        <v>0.009165921855108316</v>
       </c>
     </row>
     <row r="1058">
@@ -11020,7 +11020,7 @@
         </is>
       </c>
       <c r="B1059" t="n">
-        <v>0.3088140245749433</v>
+        <v>0.1613799442421299</v>
       </c>
     </row>
     <row r="1060">
@@ -11030,7 +11030,7 @@
         </is>
       </c>
       <c r="B1060" t="n">
-        <v>0</v>
+        <v>0.06211655010070084</v>
       </c>
     </row>
     <row r="1061">
@@ -11040,7 +11040,7 @@
         </is>
       </c>
       <c r="B1061" t="n">
-        <v>0</v>
+        <v>0.03024887477471639</v>
       </c>
     </row>
     <row r="1062">
@@ -11050,7 +11050,7 @@
         </is>
       </c>
       <c r="B1062" t="n">
-        <v>0</v>
+        <v>0.01824637034839776</v>
       </c>
     </row>
     <row r="1063">
@@ -11530,7 +11530,7 @@
         </is>
       </c>
       <c r="B1110" t="n">
-        <v>0.2375134267703939</v>
+        <v>0.08916087486108271</v>
       </c>
     </row>
     <row r="1111">
@@ -11540,7 +11540,7 @@
         </is>
       </c>
       <c r="B1111" t="n">
-        <v>0</v>
+        <v>0.0203511438562546</v>
       </c>
     </row>
     <row r="1112">
@@ -11550,7 +11550,7 @@
         </is>
       </c>
       <c r="B1112" t="n">
-        <v>0</v>
+        <v>0.008600866431933701</v>
       </c>
     </row>
     <row r="1113">
@@ -11560,7 +11560,7 @@
         </is>
       </c>
       <c r="B1113" t="n">
-        <v>0</v>
+        <v>0.005199725648036948</v>
       </c>
     </row>
     <row r="1114">
@@ -11600,7 +11600,7 @@
         </is>
       </c>
       <c r="B1117" t="n">
-        <v>0.3684874493054099</v>
+        <v>0.2564360452270001</v>
       </c>
     </row>
     <row r="1118">
@@ -11610,7 +11610,7 @@
         </is>
       </c>
       <c r="B1118" t="n">
-        <v>0</v>
+        <v>0.1210019599559433</v>
       </c>
     </row>
     <row r="1119">
@@ -11620,7 +11620,7 @@
         </is>
       </c>
       <c r="B1119" t="n">
-        <v>0</v>
+        <v>0.06497423962555407</v>
       </c>
     </row>
     <row r="1120">
@@ -11630,7 +11630,7 @@
         </is>
       </c>
       <c r="B1120" t="n">
-        <v>0</v>
+        <v>0.04125859095077777</v>
       </c>
     </row>
     <row r="1121">
@@ -12030,7 +12030,7 @@
         </is>
       </c>
       <c r="B1160" t="n">
-        <v>0.3043063921157546</v>
+        <v>0.1556309768432107</v>
       </c>
     </row>
     <row r="1161">
@@ -12040,7 +12040,7 @@
         </is>
       </c>
       <c r="B1161" t="n">
-        <v>0.3815047847190345</v>
+        <v>0.3151616911673858</v>
       </c>
     </row>
     <row r="1162">
@@ -12050,7 +12050,7 @@
         </is>
       </c>
       <c r="B1162" t="n">
-        <v>0.4158813193133258</v>
+        <v>0.4217564881908806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ready for multi-brand train
</commit_message>
<xml_diff>
--- a/estimatedParametersMean.xlsx
+++ b/estimatedParametersMean.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>311.1279424200029</v>
+        <v>311.1968628005525</v>
       </c>
     </row>
     <row r="4">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8689419050560571</v>
+        <v>0.881148574966603</v>
       </c>
     </row>
     <row r="5">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.008278819713495124</v>
+        <v>0.007999957887505975</v>
       </c>
     </row>
     <row r="6">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8.966749999999999</v>
+        <v>8.97925</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>511.0495</v>
+        <v>513.3635</v>
       </c>
     </row>
     <row r="8">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.00275</v>
+        <v>0.00075</v>
       </c>
     </row>
     <row r="9">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-283.6222918103429</v>
+        <v>-283.8146483263417</v>
       </c>
     </row>
     <row r="10">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.03646763017026558</v>
+        <v>0.03641575410125095</v>
       </c>
     </row>
     <row r="11">
@@ -535,257 +535,257 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3374536790521361</v>
+        <v>0.352383810959805</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.1</t>
+          <t>beta_seasonality_raw.1.1</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.02211474152024639</v>
+        <v>-0.03719551654179919</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.2</t>
+          <t>beta_seasonality_raw.1.2</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.02856417250873496</v>
+        <v>-0.04342567245507866</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.3</t>
+          <t>beta_seasonality_raw.1.3</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.01326969702490293</v>
+        <v>-0.02875180003855856</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.4</t>
+          <t>beta_seasonality_raw.1.4</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.003658271246392902</v>
+        <v>-0.01891615043478751</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.5</t>
+          <t>beta_seasonality_raw.1.5</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.05947439360657058</v>
+        <v>0.04406103876953447</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.6</t>
+          <t>beta_seasonality_raw.1.6</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.004388191186199099</v>
+        <v>-0.01118289042598502</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.7</t>
+          <t>beta_seasonality_raw.1.7</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.06634070783129378</v>
+        <v>0.05098268174916522</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.8</t>
+          <t>beta_seasonality_raw.1.8</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.05935582889250385</v>
+        <v>0.04389259175325202</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.9</t>
+          <t>beta_seasonality_raw.1.9</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01265902900564968</v>
+        <v>-0.002478360929340194</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.10</t>
+          <t>beta_seasonality_raw.1.10</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.02060635491626496</v>
+        <v>-0.0356565083192017</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.11</t>
+          <t>beta_seasonality_raw.1.11</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.04154363271461577</v>
+        <v>-0.05651679249744021</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.12</t>
+          <t>beta_seasonality_raw.1.12</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.0123623351383346</v>
+        <v>-0.02809794476113571</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>beta_seasonality.13</t>
+          <t>beta_tom.1</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.01785674093796598</v>
+        <v>0.02570523302675798</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>beta_tom.1</t>
+          <t>beta_laura.1</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.02579321481510268</v>
+        <v>0.01659344891885198</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>beta_laura.1</t>
+          <t>beta_lisa.1</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.01651709964113347</v>
+        <v>0.01581705634982677</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>beta_lisa.1</t>
+          <t>beta_mary.1</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.01633674507026093</v>
+        <v>0.06225989198235728</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>beta_mary.1</t>
+          <t>beta_fiona.1</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.06156441329414764</v>
+        <v>0.01535293594430449</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>beta_fiona.1</t>
+          <t>beta_marc.1</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.01634360186708455</v>
+        <v>0.02128526638451896</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>beta_marc.1</t>
+          <t>beta_alex.1</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02137262837536999</v>
+        <v>0.02928270221615438</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>beta_alex.1</t>
+          <t>beta_epros.1</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.02946300328215199</v>
+        <v>0.001312508263653732</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>beta_epros.1</t>
+          <t>beta_promotion.1</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.00130560797580111</v>
+        <v>2.434522511817783</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>beta_promotion.1</t>
+          <t>beta_distribution.1</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2.440392823847526</v>
+        <v>0.8457824255313744</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>beta_distribution.1</t>
+          <t>beta_off_trade_visibility.1</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.804995080295391</v>
+        <v>0.001742939415022856</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>beta_off_trade_visibility.1</t>
+          <t>beta_covid.1</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.001748012488490367</v>
+        <v>0.0003301209885330692</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>beta_covid.1</t>
+          <t>beta_is_last_week.1</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.000330256106229053</v>
+        <v>0.01839370544373103</v>
       </c>
     </row>
     <row r="37">
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.5447908339839141</v>
+        <v>0.5410529011361502</v>
       </c>
     </row>
     <row r="38">
@@ -805,7 +805,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.4767006261028925</v>
+        <v>0.4744293687051261</v>
       </c>
     </row>
     <row r="39">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.4817234381383302</v>
+        <v>0.4722724235903888</v>
       </c>
     </row>
     <row r="40">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.6460168984506531</v>
+        <v>0.644511841757884</v>
       </c>
     </row>
     <row r="41">
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.4300308350907416</v>
+        <v>0.439129863124513</v>
       </c>
     </row>
     <row r="42">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.4798101740032961</v>
+        <v>0.4736943260052005</v>
       </c>
     </row>
     <row r="43">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.4569162294874831</v>
+        <v>0.4592131575395766</v>
       </c>
     </row>
     <row r="44">
@@ -865,7 +865,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.9962271661266777</v>
+        <v>0.9981178803952342</v>
       </c>
     </row>
     <row r="45">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.9893732363485755</v>
+        <v>1.011741673052251</v>
       </c>
     </row>
     <row r="46">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1.007331459549819</v>
+        <v>1.006122574550032</v>
       </c>
     </row>
     <row r="47">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1.01572641570897</v>
+        <v>0.9902882566796595</v>
       </c>
     </row>
     <row r="48">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.9971933848339508</v>
+        <v>0.9974659561984749</v>
       </c>
     </row>
     <row r="49">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.9853107663112614</v>
+        <v>1.005320863225581</v>
       </c>
     </row>
     <row r="50">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.9833095697531669</v>
+        <v>0.9980493366255228</v>
       </c>
     </row>
     <row r="51">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.8852165787698876</v>
+        <v>0.8865300554216686</v>
       </c>
     </row>
     <row r="52">
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1.012195052901414</v>
+        <v>1.019753019805463</v>
       </c>
     </row>
     <row r="53">
@@ -955,7 +955,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.9854037945001689</v>
+        <v>0.9867530738552858</v>
       </c>
     </row>
     <row r="54">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.6130497367445337</v>
+        <v>0.6087008269799139</v>
       </c>
     </row>
     <row r="55">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1.102705755747095</v>
+        <v>1.091259418282038</v>
       </c>
     </row>
     <row r="56">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.9786527289494493</v>
+        <v>0.990570842911787</v>
       </c>
     </row>
     <row r="57">
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1.18515594289134</v>
+        <v>1.167867101342911</v>
       </c>
     </row>
     <row r="58">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.5271674778153413</v>
+        <v>0.5218166851106874</v>
       </c>
     </row>
     <row r="59">
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.5424714135080696</v>
+        <v>0.545326743256046</v>
       </c>
     </row>
     <row r="60">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.5293285215466842</v>
+        <v>0.5247850903755149</v>
       </c>
     </row>
     <row r="61">
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.4105622746602203</v>
+        <v>0.4061472914077259</v>
       </c>
     </row>
     <row r="62">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.5628045055788969</v>
+        <v>0.567191197351812</v>
       </c>
     </row>
     <row r="63">
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.5274899205191308</v>
+        <v>0.5259375676969282</v>
       </c>
     </row>
     <row r="64">
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.5777576765855574</v>
+        <v>0.5747822038591573</v>
       </c>
     </row>
     <row r="65">
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.1837483347823932</v>
+        <v>0.1796862432336005</v>
       </c>
     </row>
     <row r="66">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1217460613969874</v>
+        <v>0.1182293188678864</v>
       </c>
     </row>
     <row r="67">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.09617069624310388</v>
+        <v>0.09621310615518121</v>
       </c>
     </row>
     <row r="68">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.1714157108972489</v>
+        <v>0.1680581397963639</v>
       </c>
     </row>
     <row r="69">
@@ -1115,7 +1115,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.143877705821313</v>
+        <v>0.1400275065807102</v>
       </c>
     </row>
     <row r="70">
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.2043450101736257</v>
+        <v>0.2001932308388555</v>
       </c>
     </row>
     <row r="71">
@@ -1135,7 +1135,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.2316586088547112</v>
+        <v>0.2275812813718358</v>
       </c>
     </row>
     <row r="72">
@@ -1145,7 +1145,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.1869078932943646</v>
+        <v>0.1826668521903386</v>
       </c>
     </row>
     <row r="73">
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.2451413684642177</v>
+        <v>0.2415013830555686</v>
       </c>
     </row>
     <row r="74">
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.2547111018685116</v>
+        <v>0.2508508654401098</v>
       </c>
     </row>
     <row r="75">
@@ -1175,7 +1175,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.2078482718595918</v>
+        <v>0.2037098421976033</v>
       </c>
     </row>
     <row r="76">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.2215364074427271</v>
+        <v>0.2173632226388264</v>
       </c>
     </row>
     <row r="77">
@@ -1195,7 +1195,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.2376045429663754</v>
+        <v>0.2337048397516478</v>
       </c>
     </row>
     <row r="78">
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.1501330719580437</v>
+        <v>0.1471403319333858</v>
       </c>
     </row>
     <row r="79">
@@ -1215,7 +1215,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.1316302778867595</v>
+        <v>0.1294341934879156</v>
       </c>
     </row>
     <row r="80">
@@ -1225,7 +1225,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.1313464616923793</v>
+        <v>0.1284922441775941</v>
       </c>
     </row>
     <row r="81">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.03505280872324721</v>
+        <v>0.03522122586206908</v>
       </c>
     </row>
     <row r="82">
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.01192952485519514</v>
+        <v>0.01141493202442831</v>
       </c>
     </row>
     <row r="83">
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.007973666667661208</v>
+        <v>0.007459374982123204</v>
       </c>
     </row>
     <row r="84">
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.02214765040708616</v>
+        <v>0.02191889468025208</v>
       </c>
     </row>
     <row r="85">
@@ -1275,7 +1275,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.1515691012446781</v>
+        <v>0.1471195026216125</v>
       </c>
     </row>
     <row r="86">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.145457499148039</v>
+        <v>0.1419295704309567</v>
       </c>
     </row>
     <row r="87">
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.09551706595762545</v>
+        <v>0.0958333996044195</v>
       </c>
     </row>
     <row r="88">
@@ -1305,7 +1305,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.07509774067493392</v>
+        <v>0.07662980332105272</v>
       </c>
     </row>
     <row r="89">
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.05845545909972772</v>
+        <v>0.05960845154816046</v>
       </c>
     </row>
     <row r="90">
@@ -1325,7 +1325,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.02485989168770175</v>
+        <v>0.02515854636701509</v>
       </c>
     </row>
     <row r="91">
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.06355351780566201</v>
+        <v>0.06446034991969776</v>
       </c>
     </row>
     <row r="92">
@@ -1345,7 +1345,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.01785928590910537</v>
+        <v>0.01778206939584221</v>
       </c>
     </row>
     <row r="93">
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>5.221694135198664e-05</v>
+        <v>0.0001541272603679593</v>
       </c>
     </row>
     <row r="94">
@@ -1505,7 +1505,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.04715097246482843</v>
+        <v>0.04689095971965591</v>
       </c>
     </row>
     <row r="109">
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.1996666498532427</v>
+        <v>0.1954205063013397</v>
       </c>
     </row>
     <row r="110">
@@ -1525,7 +1525,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.2434511342401125</v>
+        <v>0.2393634117737549</v>
       </c>
     </row>
     <row r="111">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.2684212251180465</v>
+        <v>0.2646968261864069</v>
       </c>
     </row>
     <row r="112">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.2757544636701775</v>
+        <v>0.2721661656455768</v>
       </c>
     </row>
     <row r="113">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.2809602725516819</v>
+        <v>0.2774700036829006</v>
       </c>
     </row>
     <row r="114">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0.2834788218021944</v>
+        <v>0.2799994628006159</v>
       </c>
     </row>
     <row r="115">
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.2849679939393031</v>
+        <v>0.2815049978779319</v>
       </c>
     </row>
     <row r="116">
@@ -1585,7 +1585,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.345564270361386</v>
+        <v>0.3434587374571517</v>
       </c>
     </row>
     <row r="117">
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.2933670420176763</v>
+        <v>0.2893433722798128</v>
       </c>
     </row>
     <row r="118">
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.2674935520914742</v>
+        <v>0.2635197807596675</v>
       </c>
     </row>
     <row r="119">
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.2526209815339341</v>
+        <v>0.2487244719023388</v>
       </c>
     </row>
     <row r="120">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.2320756585875474</v>
+        <v>0.227911965895719</v>
       </c>
     </row>
     <row r="121">
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.2320756585875474</v>
+        <v>0.227911965895719</v>
       </c>
     </row>
     <row r="122">
@@ -1645,7 +1645,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>0.1064473968180101</v>
+        <v>0.1072804317304469</v>
       </c>
     </row>
     <row r="123">
@@ -1655,7 +1655,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0.03303354495426315</v>
+        <v>0.03369826933021089</v>
       </c>
     </row>
     <row r="124">
@@ -1665,7 +1665,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>6.663892861253995e-05</v>
+        <v>0.0001859813209208245</v>
       </c>
     </row>
     <row r="125">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.1562201237441485</v>
+        <v>0.1516450947925308</v>
       </c>
     </row>
     <row r="132">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.09493072810903545</v>
+        <v>0.09458437717508658</v>
       </c>
     </row>
     <row r="133">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.04198348140589481</v>
+        <v>0.04248554909912471</v>
       </c>
     </row>
     <row r="134">
@@ -1765,7 +1765,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.005902852277612571</v>
+        <v>0.005918510458036901</v>
       </c>
     </row>
     <row r="135">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.3325664444662789</v>
+        <v>0.3305971735505136</v>
       </c>
     </row>
     <row r="163">
@@ -2055,7 +2055,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.5372066071909192</v>
+        <v>0.5377854671769998</v>
       </c>
     </row>
     <row r="164">
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.5768492361988659</v>
+        <v>0.5769996205546286</v>
       </c>
     </row>
     <row r="165">
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.4335261165097288</v>
+        <v>0.4286736570529351</v>
       </c>
     </row>
     <row r="166">
@@ -2085,7 +2085,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.4782653540345654</v>
+        <v>0.4776882415364662</v>
       </c>
     </row>
     <row r="167">
@@ -2095,7 +2095,7 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.5284425165465787</v>
+        <v>0.528620763289891</v>
       </c>
     </row>
     <row r="168">
@@ -2105,7 +2105,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.581015645805114</v>
+        <v>0.5814958970082469</v>
       </c>
     </row>
     <row r="169">
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.5186613007709481</v>
+        <v>0.5165223835959351</v>
       </c>
     </row>
     <row r="170">
@@ -2125,7 +2125,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.3795237531294167</v>
+        <v>0.3755481062964135</v>
       </c>
     </row>
     <row r="171">
@@ -2135,7 +2135,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.3675838569890277</v>
+        <v>0.3658284431667021</v>
       </c>
     </row>
     <row r="172">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.3876762683338962</v>
+        <v>0.3863719833139876</v>
       </c>
     </row>
     <row r="173">
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.4192691144722133</v>
+        <v>0.4180033774030535</v>
       </c>
     </row>
     <row r="174">
@@ -2165,7 +2165,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.4471243959545768</v>
+        <v>0.446106918085575</v>
       </c>
     </row>
     <row r="175">
@@ -2175,7 +2175,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.455046327979963</v>
+        <v>0.4540566851503796</v>
       </c>
     </row>
     <row r="176">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.3029605826174131</v>
+        <v>0.2989890837816772</v>
       </c>
     </row>
     <row r="177">
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.2029941859900542</v>
+        <v>0.2007857560161083</v>
       </c>
     </row>
     <row r="178">
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.0981924021921777</v>
+        <v>0.1007906712900772</v>
       </c>
     </row>
     <row r="179">
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.2318380420412927</v>
+        <v>0.2279490999846876</v>
       </c>
     </row>
     <row r="192">
@@ -2345,7 +2345,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.3174318007473493</v>
+        <v>0.3146473335516494</v>
       </c>
     </row>
     <row r="193">
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.3792788995338222</v>
+        <v>0.3775430775807899</v>
       </c>
     </row>
     <row r="194">
@@ -2365,7 +2365,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.2388348063459056</v>
+        <v>0.2344799751626969</v>
       </c>
     </row>
     <row r="195">
@@ -2375,7 +2375,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.1314445608362446</v>
+        <v>0.1328817021979799</v>
       </c>
     </row>
     <row r="196">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.03955964581290861</v>
+        <v>0.04031639844969341</v>
       </c>
     </row>
     <row r="197">
@@ -2565,7 +2565,7 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.002748988941579851</v>
+        <v>0.002400674516948442</v>
       </c>
     </row>
     <row r="215">
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.239410514976626</v>
+        <v>0.2359401671646061</v>
       </c>
     </row>
     <row r="218">
@@ -2605,7 +2605,7 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.44954244375542</v>
+        <v>0.449259844807008</v>
       </c>
     </row>
     <row r="219">
@@ -2615,7 +2615,7 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>0.5042587788761048</v>
+        <v>0.5039375763936188</v>
       </c>
     </row>
     <row r="220">
@@ -2625,7 +2625,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.5792266809426311</v>
+        <v>0.5796351078187407</v>
       </c>
     </row>
     <row r="221">
@@ -2635,7 +2635,7 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>0.5493950248284711</v>
+        <v>0.5482629719905401</v>
       </c>
     </row>
     <row r="222">
@@ -2675,7 +2675,7 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.1441509387826475</v>
+        <v>0.1410448099378223</v>
       </c>
     </row>
     <row r="226">
@@ -2685,7 +2685,7 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.1976384969988216</v>
+        <v>0.1945528896104984</v>
       </c>
     </row>
     <row r="227">
@@ -2695,7 +2695,7 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.1504151862136098</v>
+        <v>0.1461129637051036</v>
       </c>
     </row>
     <row r="228">
@@ -2705,7 +2705,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.160007340262631</v>
+        <v>0.1559906774110116</v>
       </c>
     </row>
     <row r="229">
@@ -2715,7 +2715,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.05207437184027618</v>
+        <v>0.05104546085071197</v>
       </c>
     </row>
     <row r="230">
@@ -2725,7 +2725,7 @@
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.008055975958988399</v>
+        <v>0.008544148871614693</v>
       </c>
     </row>
     <row r="231">
@@ -2845,7 +2845,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.06008042751802065</v>
+        <v>0.0571058662280042</v>
       </c>
     </row>
     <row r="243">
@@ -2855,7 +2855,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.0430302266547496</v>
+        <v>0.04155371701763313</v>
       </c>
     </row>
     <row r="244">
@@ -2865,7 +2865,7 @@
         </is>
       </c>
       <c r="B244" t="n">
-        <v>0.01328528936249025</v>
+        <v>0.01334353916774082</v>
       </c>
     </row>
     <row r="245">
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.003531681113380753</v>
+        <v>0.003796253832679252</v>
       </c>
     </row>
     <row r="246">
@@ -3095,7 +3095,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>0.364730488395519</v>
+        <v>0.3626795506981967</v>
       </c>
     </row>
     <row r="268">
@@ -3105,7 +3105,7 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>0.4897175629985795</v>
+        <v>0.4884315238168939</v>
       </c>
     </row>
     <row r="269">
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.4641190904307927</v>
+        <v>0.4633691294511207</v>
       </c>
     </row>
     <row r="270">
@@ -3125,7 +3125,7 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.3292070243875937</v>
+        <v>0.3270287860980476</v>
       </c>
     </row>
     <row r="271">
@@ -3135,7 +3135,7 @@
         </is>
       </c>
       <c r="B271" t="n">
-        <v>0.2371675597081559</v>
+        <v>0.233113662474371</v>
       </c>
     </row>
     <row r="272">
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.1554718239637277</v>
+        <v>0.1510437093018141</v>
       </c>
     </row>
     <row r="273">
@@ -3155,7 +3155,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.1049144219290282</v>
+        <v>0.1006360474209911</v>
       </c>
     </row>
     <row r="274">
@@ -3165,7 +3165,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0.02836647753695335</v>
+        <v>0.02904293063431198</v>
       </c>
     </row>
     <row r="275">
@@ -3175,7 +3175,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.00501301925743399</v>
+        <v>0.005869141604525099</v>
       </c>
     </row>
     <row r="276">
@@ -3315,7 +3315,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>0.002144549348970316</v>
+        <v>0.002286182227274676</v>
       </c>
     </row>
     <row r="290">
@@ -3325,7 +3325,7 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>0.001043801723296301</v>
+        <v>0.001215434749737469</v>
       </c>
     </row>
     <row r="291">
@@ -3655,7 +3655,7 @@
         </is>
       </c>
       <c r="B323" t="n">
-        <v>0.2432914673061995</v>
+        <v>0.2405503977264173</v>
       </c>
     </row>
     <row r="324">
@@ -3665,7 +3665,7 @@
         </is>
       </c>
       <c r="B324" t="n">
-        <v>0.326049578812193</v>
+        <v>0.3241590729593876</v>
       </c>
     </row>
     <row r="325">
@@ -3675,7 +3675,7 @@
         </is>
       </c>
       <c r="B325" t="n">
-        <v>0.3608490379923714</v>
+        <v>0.3593467404728987</v>
       </c>
     </row>
     <row r="326">
@@ -3685,7 +3685,7 @@
         </is>
       </c>
       <c r="B326" t="n">
-        <v>0.2604708102982127</v>
+        <v>0.2572262268875589</v>
       </c>
     </row>
     <row r="327">
@@ -3695,7 +3695,7 @@
         </is>
       </c>
       <c r="B327" t="n">
-        <v>0.1259957584353473</v>
+        <v>0.1221540100119655</v>
       </c>
     </row>
     <row r="328">
@@ -3705,7 +3705,7 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>0.128473005335112</v>
+        <v>0.1243789439587231</v>
       </c>
     </row>
     <row r="329">
@@ -3715,7 +3715,7 @@
         </is>
       </c>
       <c r="B329" t="n">
-        <v>0.1251129753377384</v>
+        <v>0.1212105648790166</v>
       </c>
     </row>
     <row r="330">
@@ -3725,7 +3725,7 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>0.1394244835194954</v>
+        <v>0.1354247823100338</v>
       </c>
     </row>
     <row r="331">
@@ -3735,7 +3735,7 @@
         </is>
       </c>
       <c r="B331" t="n">
-        <v>0.1560595691981032</v>
+        <v>0.1520948404919376</v>
       </c>
     </row>
     <row r="332">
@@ -3745,7 +3745,7 @@
         </is>
       </c>
       <c r="B332" t="n">
-        <v>0.1560595691981032</v>
+        <v>0.1520948404919376</v>
       </c>
     </row>
     <row r="333">
@@ -3755,7 +3755,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>0.05134350961051817</v>
+        <v>0.05019061552410874</v>
       </c>
     </row>
     <row r="334">
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>0.0135638076072473</v>
+        <v>0.01376090113569657</v>
       </c>
     </row>
     <row r="335">
@@ -4165,7 +4165,7 @@
         </is>
       </c>
       <c r="B374" t="n">
-        <v>0.2443080842307768</v>
+        <v>0.2415720636364567</v>
       </c>
     </row>
     <row r="375">
@@ -4175,7 +4175,7 @@
         </is>
       </c>
       <c r="B375" t="n">
-        <v>0.3522589411454696</v>
+        <v>0.3504848291210003</v>
       </c>
     </row>
     <row r="376">
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="B376" t="n">
-        <v>0.3927348664402354</v>
+        <v>0.391433109751566</v>
       </c>
     </row>
     <row r="377">
@@ -4195,7 +4195,7 @@
         </is>
       </c>
       <c r="B377" t="n">
-        <v>0.4119636711939667</v>
+        <v>0.4109412821121365</v>
       </c>
     </row>
     <row r="378">
@@ -4205,7 +4205,7 @@
         </is>
       </c>
       <c r="B378" t="n">
-        <v>0.3237909981937858</v>
+        <v>0.3220210987411525</v>
       </c>
     </row>
     <row r="379">
@@ -5745,7 +5745,7 @@
         </is>
       </c>
       <c r="B532" t="n">
-        <v>0.4252673139840576</v>
+        <v>0.4271339665121227</v>
       </c>
     </row>
     <row r="533">
@@ -5755,7 +5755,7 @@
         </is>
       </c>
       <c r="B533" t="n">
-        <v>0.5227915843205899</v>
+        <v>0.5232075415338294</v>
       </c>
     </row>
     <row r="534">
@@ -5765,7 +5765,7 @@
         </is>
       </c>
       <c r="B534" t="n">
-        <v>0.5769764959594404</v>
+        <v>0.5764037350302577</v>
       </c>
     </row>
     <row r="535">
@@ -5775,7 +5775,7 @@
         </is>
       </c>
       <c r="B535" t="n">
-        <v>0.5277227040305904</v>
+        <v>0.5262653812804033</v>
       </c>
     </row>
     <row r="536">
@@ -5785,7 +5785,7 @@
         </is>
       </c>
       <c r="B536" t="n">
-        <v>0.3843053452439121</v>
+        <v>0.3877380896427804</v>
       </c>
     </row>
     <row r="537">
@@ -5795,7 +5795,7 @@
         </is>
       </c>
       <c r="B537" t="n">
-        <v>0.3086088199280084</v>
+        <v>0.311001251770111</v>
       </c>
     </row>
     <row r="538">
@@ -5805,7 +5805,7 @@
         </is>
       </c>
       <c r="B538" t="n">
-        <v>0.2226765855859062</v>
+        <v>0.2218189001473628</v>
       </c>
     </row>
     <row r="539">
@@ -5815,7 +5815,7 @@
         </is>
       </c>
       <c r="B539" t="n">
-        <v>0.1607692146387316</v>
+        <v>0.1566881385751732</v>
       </c>
     </row>
     <row r="540">
@@ -5885,7 +5885,7 @@
         </is>
       </c>
       <c r="B546" t="n">
-        <v>0.278753139125048</v>
+        <v>0.2811038604901419</v>
       </c>
     </row>
     <row r="547">
@@ -5895,7 +5895,7 @@
         </is>
       </c>
       <c r="B547" t="n">
-        <v>0.3229867257492847</v>
+        <v>0.3254504014395895</v>
       </c>
     </row>
     <row r="548">
@@ -5905,7 +5905,7 @@
         </is>
       </c>
       <c r="B548" t="n">
-        <v>0.4110215251308581</v>
+        <v>0.4146322183369269</v>
       </c>
     </row>
     <row r="549">
@@ -5915,7 +5915,7 @@
         </is>
       </c>
       <c r="B549" t="n">
-        <v>0.3373340741626363</v>
+        <v>0.3395873389864423</v>
       </c>
     </row>
     <row r="550">
@@ -5925,7 +5925,7 @@
         </is>
       </c>
       <c r="B550" t="n">
-        <v>0.2220621277403147</v>
+        <v>0.2213569861085725</v>
       </c>
     </row>
     <row r="551">
@@ -5935,7 +5935,7 @@
         </is>
       </c>
       <c r="B551" t="n">
-        <v>0.1187586253651281</v>
+        <v>0.1128185753361959</v>
       </c>
     </row>
     <row r="552">
@@ -6755,7 +6755,7 @@
         </is>
       </c>
       <c r="B633" t="n">
-        <v>0.3311281903042528</v>
+        <v>0.3340726457499245</v>
       </c>
     </row>
     <row r="634">
@@ -6765,7 +6765,7 @@
         </is>
       </c>
       <c r="B634" t="n">
-        <v>0.4971901665063521</v>
+        <v>0.5000918432827433</v>
       </c>
     </row>
     <row r="635">
@@ -6775,7 +6775,7 @@
         </is>
       </c>
       <c r="B635" t="n">
-        <v>0.5494043209747678</v>
+        <v>0.5513938197180973</v>
       </c>
     </row>
     <row r="636">
@@ -6785,7 +6785,7 @@
         </is>
       </c>
       <c r="B636" t="n">
-        <v>0.491484721003273</v>
+        <v>0.495764249807584</v>
       </c>
     </row>
     <row r="637">
@@ -6795,7 +6795,7 @@
         </is>
       </c>
       <c r="B637" t="n">
-        <v>0.5588760821113817</v>
+        <v>0.5606837070631576</v>
       </c>
     </row>
     <row r="638">
@@ -6805,7 +6805,7 @@
         </is>
       </c>
       <c r="B638" t="n">
-        <v>0.5740560640743022</v>
+        <v>0.5755927974352586</v>
       </c>
     </row>
     <row r="639">
@@ -6815,7 +6815,7 @@
         </is>
       </c>
       <c r="B639" t="n">
-        <v>0.5799356934480897</v>
+        <v>0.5814566292102528</v>
       </c>
     </row>
     <row r="640">
@@ -6825,7 +6825,7 @@
         </is>
       </c>
       <c r="B640" t="n">
-        <v>0.5524981568249759</v>
+        <v>0.5555153531139704</v>
       </c>
     </row>
     <row r="641">
@@ -6835,7 +6835,7 @@
         </is>
       </c>
       <c r="B641" t="n">
-        <v>0.4789884831403826</v>
+        <v>0.4839511483977341</v>
       </c>
     </row>
     <row r="642">
@@ -6845,7 +6845,7 @@
         </is>
       </c>
       <c r="B642" t="n">
-        <v>0.495064911976051</v>
+        <v>0.4983464205908488</v>
       </c>
     </row>
     <row r="643">
@@ -6855,7 +6855,7 @@
         </is>
       </c>
       <c r="B643" t="n">
-        <v>0.5051086186622001</v>
+        <v>0.5080553355235348</v>
       </c>
     </row>
     <row r="644">
@@ -6865,7 +6865,7 @@
         </is>
       </c>
       <c r="B644" t="n">
-        <v>0.5225849446502366</v>
+        <v>0.5253715118099164</v>
       </c>
     </row>
     <row r="645">
@@ -6875,7 +6875,7 @@
         </is>
       </c>
       <c r="B645" t="n">
-        <v>0.5354290338174705</v>
+        <v>0.5381039307939951</v>
       </c>
     </row>
     <row r="646">
@@ -6885,7 +6885,7 @@
         </is>
       </c>
       <c r="B646" t="n">
-        <v>0.5369629244299364</v>
+        <v>0.5396365695839284</v>
       </c>
     </row>
     <row r="647">
@@ -6895,7 +6895,7 @@
         </is>
       </c>
       <c r="B647" t="n">
-        <v>0.4640401645280053</v>
+        <v>0.468836182563189</v>
       </c>
     </row>
     <row r="648">
@@ -6905,7 +6905,7 @@
         </is>
       </c>
       <c r="B648" t="n">
-        <v>0.3677450150010537</v>
+        <v>0.3702209550127529</v>
       </c>
     </row>
     <row r="649">
@@ -6915,7 +6915,7 @@
         </is>
       </c>
       <c r="B649" t="n">
-        <v>0.2282912769817842</v>
+        <v>0.2272804853040307</v>
       </c>
     </row>
     <row r="650">
@@ -7305,7 +7305,7 @@
         </is>
       </c>
       <c r="B688" t="n">
-        <v>0.343820536034275</v>
+        <v>0.3469070518865769</v>
       </c>
     </row>
     <row r="689">
@@ -7315,7 +7315,7 @@
         </is>
       </c>
       <c r="B689" t="n">
-        <v>0.5200297331029717</v>
+        <v>0.5224163493635126</v>
       </c>
     </row>
     <row r="690">
@@ -7325,7 +7325,7 @@
         </is>
       </c>
       <c r="B690" t="n">
-        <v>0.5422968498035853</v>
+        <v>0.5446396527711209</v>
       </c>
     </row>
     <row r="691">
@@ -7335,7 +7335,7 @@
         </is>
       </c>
       <c r="B691" t="n">
-        <v>0.5798551117489593</v>
+        <v>0.5812233094567724</v>
       </c>
     </row>
     <row r="692">
@@ -7345,7 +7345,7 @@
         </is>
       </c>
       <c r="B692" t="n">
-        <v>0.5927562990424765</v>
+        <v>0.5939688627641958</v>
       </c>
     </row>
     <row r="693">
@@ -7375,7 +7375,7 @@
         </is>
       </c>
       <c r="B695" t="n">
-        <v>0.06791744986715327</v>
+        <v>0.06864609868474801</v>
       </c>
     </row>
     <row r="696">
@@ -7385,7 +7385,7 @@
         </is>
       </c>
       <c r="B696" t="n">
-        <v>0.00785343610948311</v>
+        <v>0.008757358749133594</v>
       </c>
     </row>
     <row r="697">
@@ -7395,7 +7395,7 @@
         </is>
       </c>
       <c r="B697" t="n">
-        <v>0.00285846026128585</v>
+        <v>0.003211270590413824</v>
       </c>
     </row>
     <row r="698">
@@ -7405,7 +7405,7 @@
         </is>
       </c>
       <c r="B698" t="n">
-        <v>0.001683401687863768</v>
+        <v>0.001875157127629781</v>
       </c>
     </row>
     <row r="699">
@@ -7775,7 +7775,7 @@
         </is>
       </c>
       <c r="B735" t="n">
-        <v>0.2031954153493443</v>
+        <v>0.1998450727360368</v>
       </c>
     </row>
     <row r="736">
@@ -7785,7 +7785,7 @@
         </is>
       </c>
       <c r="B736" t="n">
-        <v>0.404726115050541</v>
+        <v>0.4018092870655192</v>
       </c>
     </row>
     <row r="737">
@@ -7795,7 +7795,7 @@
         </is>
       </c>
       <c r="B737" t="n">
-        <v>0.4338266400368311</v>
+        <v>0.4327477224500323</v>
       </c>
     </row>
     <row r="738">
@@ -7805,7 +7805,7 @@
         </is>
       </c>
       <c r="B738" t="n">
-        <v>0.2981547768240249</v>
+        <v>0.297875017694953</v>
       </c>
     </row>
     <row r="739">
@@ -7815,7 +7815,7 @@
         </is>
       </c>
       <c r="B739" t="n">
-        <v>0.2765104893321669</v>
+        <v>0.2754640477568087</v>
       </c>
     </row>
     <row r="740">
@@ -7825,7 +7825,7 @@
         </is>
       </c>
       <c r="B740" t="n">
-        <v>0.3070460728730134</v>
+        <v>0.3046908353549272</v>
       </c>
     </row>
     <row r="741">
@@ -7835,7 +7835,7 @@
         </is>
       </c>
       <c r="B741" t="n">
-        <v>0.3691352132538098</v>
+        <v>0.3666875246261954</v>
       </c>
     </row>
     <row r="742">
@@ -7845,7 +7845,7 @@
         </is>
       </c>
       <c r="B742" t="n">
-        <v>0.3319947517797722</v>
+        <v>0.3302763883301695</v>
       </c>
     </row>
     <row r="743">
@@ -7855,7 +7855,7 @@
         </is>
       </c>
       <c r="B743" t="n">
-        <v>0.2691938840779743</v>
+        <v>0.2677198249856016</v>
       </c>
     </row>
     <row r="744">
@@ -7865,7 +7865,7 @@
         </is>
       </c>
       <c r="B744" t="n">
-        <v>0.176792467454782</v>
+        <v>0.1771438216477735</v>
       </c>
     </row>
     <row r="745">
@@ -7875,7 +7875,7 @@
         </is>
       </c>
       <c r="B745" t="n">
-        <v>0.1339651609387834</v>
+        <v>0.134317135542905</v>
       </c>
     </row>
     <row r="746">
@@ -7885,7 +7885,7 @@
         </is>
       </c>
       <c r="B746" t="n">
-        <v>0.04293740782173455</v>
+        <v>0.04348026049198152</v>
       </c>
     </row>
     <row r="747">
@@ -7895,7 +7895,7 @@
         </is>
       </c>
       <c r="B747" t="n">
-        <v>0.00738761084315604</v>
+        <v>0.008208898852984318</v>
       </c>
     </row>
     <row r="748">
@@ -7905,7 +7905,7 @@
         </is>
       </c>
       <c r="B748" t="n">
-        <v>0.0003593950575924431</v>
+        <v>0.0004582946949224232</v>
       </c>
     </row>
     <row r="749">
@@ -7955,7 +7955,7 @@
         </is>
       </c>
       <c r="B753" t="n">
-        <v>0.2646846609508027</v>
+        <v>0.2604370236154114</v>
       </c>
     </row>
     <row r="754">
@@ -7965,7 +7965,7 @@
         </is>
       </c>
       <c r="B754" t="n">
-        <v>0.1265091810023244</v>
+        <v>0.1261720615733385</v>
       </c>
     </row>
     <row r="755">
@@ -7975,7 +7975,7 @@
         </is>
       </c>
       <c r="B755" t="n">
-        <v>0.06637416181924022</v>
+        <v>0.06721836830513228</v>
       </c>
     </row>
     <row r="756">
@@ -7985,7 +7985,7 @@
         </is>
       </c>
       <c r="B756" t="n">
-        <v>0.03944469785963364</v>
+        <v>0.04056550768429425</v>
       </c>
     </row>
     <row r="757">
@@ -8005,7 +8005,7 @@
         </is>
       </c>
       <c r="B758" t="n">
-        <v>0.0639969340798608</v>
+        <v>0.06482402894740236</v>
       </c>
     </row>
     <row r="759">
@@ -8015,7 +8015,7 @@
         </is>
       </c>
       <c r="B759" t="n">
-        <v>0.00651107327171248</v>
+        <v>0.007258940923650086</v>
       </c>
     </row>
     <row r="760">
@@ -8025,7 +8025,7 @@
         </is>
       </c>
       <c r="B760" t="n">
-        <v>0.002355562741413229</v>
+        <v>0.002617404778601767</v>
       </c>
     </row>
     <row r="761">
@@ -8035,7 +8035,7 @@
         </is>
       </c>
       <c r="B761" t="n">
-        <v>0.001465284488765904</v>
+        <v>0.001557980738945299</v>
       </c>
     </row>
     <row r="762">
@@ -8555,7 +8555,7 @@
         </is>
       </c>
       <c r="B813" t="n">
-        <v>0.1056686585346069</v>
+        <v>0.105219589101956</v>
       </c>
     </row>
     <row r="814">
@@ -8565,7 +8565,7 @@
         </is>
       </c>
       <c r="B814" t="n">
-        <v>0.0267921771599061</v>
+        <v>0.0272218739065253</v>
       </c>
     </row>
     <row r="815">
@@ -8575,7 +8575,7 @@
         </is>
       </c>
       <c r="B815" t="n">
-        <v>0.0100434738254217</v>
+        <v>0.01109314459202164</v>
       </c>
     </row>
     <row r="816">
@@ -8585,7 +8585,7 @@
         </is>
       </c>
       <c r="B816" t="n">
-        <v>0.005713862463346877</v>
+        <v>0.006368211600722737</v>
       </c>
     </row>
     <row r="817">
@@ -8875,7 +8875,7 @@
         </is>
       </c>
       <c r="B845" t="n">
-        <v>0.3119099080944409</v>
+        <v>0.3075566234903341</v>
       </c>
     </row>
     <row r="846">
@@ -8885,7 +8885,7 @@
         </is>
       </c>
       <c r="B846" t="n">
-        <v>0.2333741502218774</v>
+        <v>0.2307460227492393</v>
       </c>
     </row>
     <row r="847">
@@ -8895,7 +8895,7 @@
         </is>
       </c>
       <c r="B847" t="n">
-        <v>0.3791437090832266</v>
+        <v>0.3768060400303619</v>
       </c>
     </row>
     <row r="848">
@@ -8905,7 +8905,7 @@
         </is>
       </c>
       <c r="B848" t="n">
-        <v>0.3344525692457483</v>
+        <v>0.3331082175883852</v>
       </c>
     </row>
     <row r="849">
@@ -8915,7 +8915,7 @@
         </is>
       </c>
       <c r="B849" t="n">
-        <v>0.452012781380992</v>
+        <v>0.4508911694582797</v>
       </c>
     </row>
     <row r="850">
@@ -8945,7 +8945,7 @@
         </is>
       </c>
       <c r="B852" t="n">
-        <v>0.3690491220068489</v>
+        <v>0.3665302371744853</v>
       </c>
     </row>
     <row r="853">
@@ -8955,7 +8955,7 @@
         </is>
       </c>
       <c r="B853" t="n">
-        <v>0.207190751980768</v>
+        <v>0.2014626207137298</v>
       </c>
     </row>
     <row r="854">
@@ -8965,7 +8965,7 @@
         </is>
       </c>
       <c r="B854" t="n">
-        <v>0.1329858839616926</v>
+        <v>0.1311655494625559</v>
       </c>
     </row>
     <row r="855">
@@ -8975,7 +8975,7 @@
         </is>
       </c>
       <c r="B855" t="n">
-        <v>0.3904974446951198</v>
+        <v>0.387231217327665</v>
       </c>
     </row>
     <row r="856">
@@ -8985,7 +8985,7 @@
         </is>
       </c>
       <c r="B856" t="n">
-        <v>0.2552000937596786</v>
+        <v>0.2492656708060031</v>
       </c>
     </row>
     <row r="857">
@@ -8995,7 +8995,7 @@
         </is>
       </c>
       <c r="B857" t="n">
-        <v>0.1295772150501465</v>
+        <v>0.1284612830877654</v>
       </c>
     </row>
     <row r="858">
@@ -9005,7 +9005,7 @@
         </is>
       </c>
       <c r="B858" t="n">
-        <v>0.06543932937634943</v>
+        <v>0.06775855375189767</v>
       </c>
     </row>
     <row r="859">
@@ -9395,7 +9395,7 @@
         </is>
       </c>
       <c r="B897" t="n">
-        <v>0.4959086427772496</v>
+        <v>0.495256865649527</v>
       </c>
     </row>
     <row r="898">
@@ -9405,7 +9405,7 @@
         </is>
       </c>
       <c r="B898" t="n">
-        <v>0.3198807110421298</v>
+        <v>0.3123560596631339</v>
       </c>
     </row>
     <row r="899">
@@ -9415,7 +9415,7 @@
         </is>
       </c>
       <c r="B899" t="n">
-        <v>0.1902143355235366</v>
+        <v>0.1872289058512366</v>
       </c>
     </row>
     <row r="900">
@@ -9425,7 +9425,7 @@
         </is>
       </c>
       <c r="B900" t="n">
-        <v>0.4246492702386019</v>
+        <v>0.4214168442682609</v>
       </c>
     </row>
     <row r="901">
@@ -9435,7 +9435,7 @@
         </is>
       </c>
       <c r="B901" t="n">
-        <v>0.2068624358775559</v>
+        <v>0.2011112826845796</v>
       </c>
     </row>
     <row r="902">
@@ -9445,7 +9445,7 @@
         </is>
       </c>
       <c r="B902" t="n">
-        <v>0.4646033341337004</v>
+        <v>0.4621476641049356</v>
       </c>
     </row>
     <row r="903">
@@ -9455,7 +9455,7 @@
         </is>
       </c>
       <c r="B903" t="n">
-        <v>0.2929802067633906</v>
+        <v>0.2859820978903881</v>
       </c>
     </row>
     <row r="904">
@@ -9465,7 +9465,7 @@
         </is>
       </c>
       <c r="B904" t="n">
-        <v>0.1370998432848991</v>
+        <v>0.1358940673164913</v>
       </c>
     </row>
     <row r="905">
@@ -9475,7 +9475,7 @@
         </is>
       </c>
       <c r="B905" t="n">
-        <v>0.07706414292449575</v>
+        <v>0.07918435954152579</v>
       </c>
     </row>
     <row r="906">
@@ -9485,7 +9485,7 @@
         </is>
       </c>
       <c r="B906" t="n">
-        <v>0.1940951999322152</v>
+        <v>0.1900824979682481</v>
       </c>
     </row>
     <row r="907">
@@ -9495,7 +9495,7 @@
         </is>
       </c>
       <c r="B907" t="n">
-        <v>0.2838011775128131</v>
+        <v>0.2795356121232973</v>
       </c>
     </row>
     <row r="908">
@@ -9505,7 +9505,7 @@
         </is>
       </c>
       <c r="B908" t="n">
-        <v>0.1402159803496862</v>
+        <v>0.13787632008281</v>
       </c>
     </row>
     <row r="909">
@@ -9515,7 +9515,7 @@
         </is>
       </c>
       <c r="B909" t="n">
-        <v>0.06582374530489989</v>
+        <v>0.06792835198798221</v>
       </c>
     </row>
     <row r="910">
@@ -9525,7 +9525,7 @@
         </is>
       </c>
       <c r="B910" t="n">
-        <v>0.0158292621724062</v>
+        <v>0.0170953775548633</v>
       </c>
     </row>
     <row r="911">
@@ -9935,7 +9935,7 @@
         </is>
       </c>
       <c r="B951" t="n">
-        <v>0.5463751782588889</v>
+        <v>0.5467699341980238</v>
       </c>
     </row>
     <row r="952">
@@ -9945,7 +9945,7 @@
         </is>
       </c>
       <c r="B952" t="n">
-        <v>0.3732603333130348</v>
+        <v>0.365114326878241</v>
       </c>
     </row>
     <row r="953">
@@ -9955,7 +9955,7 @@
         </is>
       </c>
       <c r="B953" t="n">
-        <v>0.2344312931521871</v>
+        <v>0.2303441035031171</v>
       </c>
     </row>
     <row r="954">
@@ -9965,7 +9965,7 @@
         </is>
       </c>
       <c r="B954" t="n">
-        <v>0.1443471935657898</v>
+        <v>0.1443007255905588</v>
       </c>
     </row>
     <row r="955">
@@ -9975,7 +9975,7 @@
         </is>
       </c>
       <c r="B955" t="n">
-        <v>0.2841449503928144</v>
+        <v>0.2807278987119607</v>
       </c>
     </row>
     <row r="956">
@@ -9985,7 +9985,7 @@
         </is>
       </c>
       <c r="B956" t="n">
-        <v>0.214887547089271</v>
+        <v>0.2095839635817923</v>
       </c>
     </row>
     <row r="957">
@@ -9995,7 +9995,7 @@
         </is>
       </c>
       <c r="B957" t="n">
-        <v>0.3600552683775524</v>
+        <v>0.3562234908593603</v>
       </c>
     </row>
     <row r="958">
@@ -10005,7 +10005,7 @@
         </is>
       </c>
       <c r="B958" t="n">
-        <v>0.4765410571932591</v>
+        <v>0.4735967642413101</v>
       </c>
     </row>
     <row r="959">
@@ -10015,7 +10015,7 @@
         </is>
       </c>
       <c r="B959" t="n">
-        <v>0.291789825788513</v>
+        <v>0.284760173466332</v>
       </c>
     </row>
     <row r="960">
@@ -10025,7 +10025,7 @@
         </is>
       </c>
       <c r="B960" t="n">
-        <v>0.1672033454263122</v>
+        <v>0.1655783594941048</v>
       </c>
     </row>
     <row r="961">
@@ -10035,7 +10035,7 @@
         </is>
       </c>
       <c r="B961" t="n">
-        <v>0.06816197334947011</v>
+        <v>0.07057331128070422</v>
       </c>
     </row>
     <row r="962">
@@ -10045,7 +10045,7 @@
         </is>
       </c>
       <c r="B962" t="n">
-        <v>0.07849833138554078</v>
+        <v>0.07614958665683155</v>
       </c>
     </row>
     <row r="963">
@@ -10055,7 +10055,7 @@
         </is>
       </c>
       <c r="B963" t="n">
-        <v>0.004022695186904604</v>
+        <v>0.004322095144638301</v>
       </c>
     </row>
     <row r="964">
@@ -10065,7 +10065,7 @@
         </is>
       </c>
       <c r="B964" t="n">
-        <v>0.00192149390103429</v>
+        <v>0.001130640255595332</v>
       </c>
     </row>
     <row r="965">
@@ -10075,7 +10075,7 @@
         </is>
       </c>
       <c r="B965" t="n">
-        <v>0.001249500904774336</v>
+        <v>0.0005106487652641016</v>
       </c>
     </row>
     <row r="966">
@@ -10455,7 +10455,7 @@
         </is>
       </c>
       <c r="B1003" t="n">
-        <v>0.05317302550424746</v>
+        <v>0.05139390473299785</v>
       </c>
     </row>
     <row r="1004">
@@ -10465,7 +10465,7 @@
         </is>
       </c>
       <c r="B1004" t="n">
-        <v>0.001241811206532488</v>
+        <v>0.0007211017937367429</v>
       </c>
     </row>
     <row r="1005">
@@ -10475,7 +10475,7 @@
         </is>
       </c>
       <c r="B1005" t="n">
-        <v>0.4871089904263126</v>
+        <v>0.4860787238227318</v>
       </c>
     </row>
     <row r="1006">
@@ -10485,7 +10485,7 @@
         </is>
       </c>
       <c r="B1006" t="n">
-        <v>0.3116376648250134</v>
+        <v>0.3043025662712667</v>
       </c>
     </row>
     <row r="1007">
@@ -10975,7 +10975,7 @@
         </is>
       </c>
       <c r="B1055" t="n">
-        <v>0.1127498082268158</v>
+        <v>0.1140064327718824</v>
       </c>
     </row>
     <row r="1056">
@@ -10985,7 +10985,7 @@
         </is>
       </c>
       <c r="B1056" t="n">
-        <v>0.03090838276319389</v>
+        <v>0.03138203945696495</v>
       </c>
     </row>
     <row r="1057">
@@ -10995,7 +10995,7 @@
         </is>
       </c>
       <c r="B1057" t="n">
-        <v>0.01285178906483339</v>
+        <v>0.01200934781565227</v>
       </c>
     </row>
     <row r="1058">
@@ -11005,7 +11005,7 @@
         </is>
       </c>
       <c r="B1058" t="n">
-        <v>0.007458940125176217</v>
+        <v>0.006587560498841853</v>
       </c>
     </row>
     <row r="1059">
@@ -11025,7 +11025,7 @@
         </is>
       </c>
       <c r="B1060" t="n">
-        <v>0.1594491201279085</v>
+        <v>0.160648914609728</v>
       </c>
     </row>
     <row r="1061">
@@ -11035,7 +11035,7 @@
         </is>
       </c>
       <c r="B1061" t="n">
-        <v>0.05870183523964496</v>
+        <v>0.06000709669771671</v>
       </c>
     </row>
     <row r="1062">
@@ -11045,7 +11045,7 @@
         </is>
       </c>
       <c r="B1062" t="n">
-        <v>0.02623858264249755</v>
+        <v>0.02526325922166542</v>
       </c>
     </row>
     <row r="1063">
@@ -11055,7 +11055,7 @@
         </is>
       </c>
       <c r="B1063" t="n">
-        <v>0.01521796553271285</v>
+        <v>0.01422904102546266</v>
       </c>
     </row>
     <row r="1064">
@@ -11535,7 +11535,7 @@
         </is>
       </c>
       <c r="B1111" t="n">
-        <v>0.08684433905733283</v>
+        <v>0.08802433363507586</v>
       </c>
     </row>
     <row r="1112">
@@ -11545,7 +11545,7 @@
         </is>
       </c>
       <c r="B1112" t="n">
-        <v>0.01761019691149405</v>
+        <v>0.01720258936641949</v>
       </c>
     </row>
     <row r="1113">
@@ -11555,7 +11555,7 @@
         </is>
       </c>
       <c r="B1113" t="n">
-        <v>0.007093892817974703</v>
+        <v>0.006341324302114744</v>
       </c>
     </row>
     <row r="1114">
@@ -11565,7 +11565,7 @@
         </is>
       </c>
       <c r="B1114" t="n">
-        <v>0.004202004292185226</v>
+        <v>0.00342754212649277</v>
       </c>
     </row>
     <row r="1115">
@@ -11605,7 +11605,7 @@
         </is>
       </c>
       <c r="B1118" t="n">
-        <v>0.2548147502657999</v>
+        <v>0.255819984686842</v>
       </c>
     </row>
     <row r="1119">
@@ -11615,7 +11615,7 @@
         </is>
       </c>
       <c r="B1119" t="n">
-        <v>0.1172146289886103</v>
+        <v>0.1188899960556521</v>
       </c>
     </row>
     <row r="1120">
@@ -11625,7 +11625,7 @@
         </is>
       </c>
       <c r="B1120" t="n">
-        <v>0.05889357796155546</v>
+        <v>0.05973844838755289</v>
       </c>
     </row>
     <row r="1121">
@@ -11635,7 +11635,7 @@
         </is>
       </c>
       <c r="B1121" t="n">
-        <v>0.0356648930664147</v>
+        <v>0.03441764478919358</v>
       </c>
     </row>
     <row r="1122">
@@ -12035,7 +12035,7 @@
         </is>
       </c>
       <c r="B1161" t="n">
-        <v>0.1536757171741793</v>
+        <v>0.1548931644437942</v>
       </c>
     </row>
     <row r="1162">
@@ -12045,7 +12045,7 @@
         </is>
       </c>
       <c r="B1162" t="n">
-        <v>0.3126219456895849</v>
+        <v>0.3143779453288642</v>
       </c>
     </row>
     <row r="1163">
@@ -12055,7 +12055,7 @@
         </is>
       </c>
       <c r="B1163" t="n">
-        <v>0.41872990212883</v>
+        <v>0.4211777335110576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>